<commit_message>
UPDATE: fitur pencarian berdasarkan kolom tertentu
</commit_message>
<xml_diff>
--- a/uploads/dataset.xlsx
+++ b/uploads/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iqbal al-ayyubi\Documents\upn-jatim\semester 3\Statkom\Review Jurnal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{E2F9A455-4F1A-4481-AD6F-1A78AEDCC0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625848C1-B3E8-40E3-A8FF-4AD2079F6C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATASET" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="TESTING" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1036,7 +1035,16 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="16" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="24" xfId="25" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1048,19 +1056,10 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="24" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="24" xfId="25" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="19" applyBorder="1" applyAlignment="1">
@@ -3211,8 +3210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D884DC29-9C63-4ED2-98E5-F89FE5DACB23}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3906,8 +3905,8 @@
         <v>7/11</v>
       </c>
       <c r="K25" s="2">
-        <f>ROUNDDOWN(D25/$B$50,2)</f>
-        <v>0.77</v>
+        <f>ROUNDDOWN(D25/$B$51,2)</f>
+        <v>0.63</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -3941,8 +3940,8 @@
         <v>4/11</v>
       </c>
       <c r="K26" s="2">
-        <f>ROUNDDOWN(D26/$B$50,2)</f>
-        <v>0.44</v>
+        <f>ROUNDDOWN(D26/$B$51,2)</f>
+        <v>0.36</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -4293,8 +4292,8 @@
         <v>7</v>
       </c>
       <c r="D41" s="2">
-        <f>COUNTIFS(Table2[A4],B41,Table2[Kelas],$D$40)</f>
-        <v>1</v>
+        <f>COUNTIFS(Table2[A5],B41,Table2[Kelas],$D$40)</f>
+        <v>6</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="35" t="s">
@@ -4313,11 +4312,11 @@
       </c>
       <c r="J41" s="2" t="str">
         <f>CONCATENATE(D41,"/",$B$51)</f>
-        <v>1/11</v>
+        <v>6/11</v>
       </c>
       <c r="K41" s="2">
         <f>ROUNDDOWN(D41/$B$51,2)</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
@@ -4330,8 +4329,8 @@
         <v>2</v>
       </c>
       <c r="D42" s="2">
-        <f>COUNTIFS(Table2[A4],B42,Table2[Kelas],$D$40)</f>
-        <v>10</v>
+        <f>COUNTIFS(Table2[A5],B42,Table2[Kelas],$D$40)</f>
+        <v>5</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="35"/>
@@ -4348,11 +4347,11 @@
       </c>
       <c r="J42" s="2" t="str">
         <f>CONCATENATE(D42,"/",$B$51)</f>
-        <v>10/11</v>
+        <v>5/11</v>
       </c>
       <c r="K42" s="2">
         <f>ROUNDDOWN(D42/$B$51,2)</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
@@ -4906,10 +4905,10 @@
       <c r="H67" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J67" s="47" t="s">
+      <c r="J67" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="K67" s="47"/>
+      <c r="K67" s="49"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="7">
@@ -4936,8 +4935,8 @@
       <c r="H68" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J68" s="47"/>
-      <c r="K68" s="47"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="49"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="7">
@@ -4964,11 +4963,11 @@
       <c r="H69" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J69" s="48">
-        <f>16/20*100</f>
-        <v>80</v>
-      </c>
-      <c r="K69" s="48"/>
+      <c r="J69" s="50">
+        <f>17/20*100</f>
+        <v>85</v>
+      </c>
+      <c r="K69" s="50"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="7">
@@ -4995,8 +4994,8 @@
       <c r="H70" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J70" s="48"/>
-      <c r="K70" s="48"/>
+      <c r="J70" s="50"/>
+      <c r="K70" s="50"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="7">
@@ -5023,8 +5022,8 @@
       <c r="H71" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J71" s="48"/>
-      <c r="K71" s="48"/>
+      <c r="J71" s="50"/>
+      <c r="K71" s="50"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="7">
@@ -5051,8 +5050,8 @@
       <c r="H72" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J72" s="48"/>
-      <c r="K72" s="48"/>
+      <c r="J72" s="50"/>
+      <c r="K72" s="50"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="7">
@@ -5206,9 +5205,9 @@
       <c r="H80" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="50" t="str">
+      <c r="I80" s="45" t="str">
         <f>IF(H81&gt;H82,B81,B82)</f>
-        <v>Ya</v>
+        <v>Tidak</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
@@ -5242,7 +5241,7 @@
         <f>PRODUCT(C81:G81)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I81" s="50"/>
+      <c r="I81" s="45"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="55"/>
@@ -5251,7 +5250,7 @@
       </c>
       <c r="C82" s="20">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D82" s="20">
         <f>K30</f>
@@ -5263,7 +5262,7 @@
       </c>
       <c r="F82" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G82" s="20">
         <f>K47</f>
@@ -5271,15 +5270,15 @@
       </c>
       <c r="H82" s="20">
         <f>PRODUCT(C82:G82)*$C$51</f>
-        <v>6.6686004000000012E-3</v>
-      </c>
-      <c r="I82" s="50"/>
+        <v>3.2736765600000009E-2</v>
+      </c>
+      <c r="I82" s="45"/>
     </row>
     <row r="83" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="41">
         <v>2</v>
       </c>
-      <c r="B83" s="42"/>
+      <c r="B83" s="43"/>
       <c r="C83" s="19" t="s">
         <v>1</v>
       </c>
@@ -5298,7 +5297,7 @@
       <c r="H83" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I83" s="50" t="str">
+      <c r="I83" s="44" t="str">
         <f>IF(H84&gt;H85,B84,B85)</f>
         <v>Ya</v>
       </c>
@@ -5334,16 +5333,16 @@
         <f>PRODUCT(C84:G84)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I84" s="50"/>
+      <c r="I84" s="44"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" s="46"/>
+      <c r="A85" s="42"/>
       <c r="B85" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C85" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D85" s="20">
         <f>K30</f>
@@ -5355,7 +5354,7 @@
       </c>
       <c r="F85" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G85" s="20">
         <f>K47</f>
@@ -5363,15 +5362,15 @@
       </c>
       <c r="H85" s="20">
         <f>PRODUCT(C85:G85)*$C$51</f>
-        <v>3.8106287999999998E-3</v>
-      </c>
-      <c r="I85" s="50"/>
+        <v>1.8706723200000004E-2</v>
+      </c>
+      <c r="I85" s="44"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="41">
         <v>3</v>
       </c>
-      <c r="B86" s="42"/>
+      <c r="B86" s="43"/>
       <c r="C86" s="19" t="s">
         <v>1</v>
       </c>
@@ -5390,7 +5389,7 @@
       <c r="H86" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I86" s="50" t="str">
+      <c r="I86" s="44" t="str">
         <f>IF(H87&gt;H88,B87,B88)</f>
         <v>Ya</v>
       </c>
@@ -5426,16 +5425,16 @@
         <f>PRODUCT(C87:G87)*$C$50</f>
         <v>3.0438639000000003E-2</v>
       </c>
-      <c r="I87" s="50"/>
+      <c r="I87" s="44"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="46"/>
+      <c r="A88" s="42"/>
       <c r="B88" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C88" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D88" s="20">
         <f>K31</f>
@@ -5447,7 +5446,7 @@
       </c>
       <c r="F88" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G88" s="20">
         <f>K47</f>
@@ -5455,15 +5454,15 @@
       </c>
       <c r="H88" s="20">
         <f>PRODUCT(C88:G88)*$C$51</f>
-        <v>1.9053144E-4</v>
-      </c>
-      <c r="I88" s="50"/>
+        <v>9.3533616000000016E-4</v>
+      </c>
+      <c r="I88" s="44"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="41">
         <v>4</v>
       </c>
-      <c r="B89" s="42"/>
+      <c r="B89" s="43"/>
       <c r="C89" s="19" t="s">
         <v>0</v>
       </c>
@@ -5482,7 +5481,7 @@
       <c r="H89" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I89" s="50" t="str">
+      <c r="I89" s="44" t="str">
         <f>IF(H90&gt;H91,B90,B91)</f>
         <v>Tidak</v>
       </c>
@@ -5518,16 +5517,16 @@
         <f>PRODUCT(C90:G90)*$C$50</f>
         <v>2.4350911200000003E-3</v>
       </c>
-      <c r="I90" s="50"/>
+      <c r="I90" s="44"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91" s="46"/>
+      <c r="A91" s="42"/>
       <c r="B91" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C91" s="24">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D91" s="24">
         <f>K32</f>
@@ -5539,7 +5538,7 @@
       </c>
       <c r="F91" s="24">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G91" s="24">
         <f>K46</f>
@@ -5547,15 +5546,15 @@
       </c>
       <c r="H91" s="20">
         <f>PRODUCT(C91:G91)*$C$51</f>
-        <v>3.8900169000000004E-3</v>
-      </c>
-      <c r="I91" s="50"/>
+        <v>1.9096446600000004E-2</v>
+      </c>
+      <c r="I91" s="44"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="41">
         <v>5</v>
       </c>
-      <c r="B92" s="42"/>
+      <c r="B92" s="43"/>
       <c r="C92" s="19" t="s">
         <v>0</v>
       </c>
@@ -5574,7 +5573,7 @@
       <c r="H92" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I92" s="50" t="str">
+      <c r="I92" s="44" t="str">
         <f>IF(H93&gt;H94,B93,B94)</f>
         <v>Ya</v>
       </c>
@@ -5610,16 +5609,16 @@
         <f>PRODUCT(C93:G93)*$C$50</f>
         <v>3.8048298750000004E-3</v>
       </c>
-      <c r="I93" s="50"/>
+      <c r="I93" s="44"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94" s="46"/>
+      <c r="A94" s="42"/>
       <c r="B94" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C94" s="24">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D94" s="24">
         <f>K32</f>
@@ -5631,7 +5630,7 @@
       </c>
       <c r="F94" s="24">
         <f>K42</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="G94" s="24">
         <f>K47</f>
@@ -5639,15 +5638,15 @@
       </c>
       <c r="H94" s="20">
         <f>PRODUCT(C94:G94)*$C$51</f>
-        <v>2.2228668000000003E-3</v>
-      </c>
-      <c r="I94" s="50"/>
+        <v>9.0935460000000001E-4</v>
+      </c>
+      <c r="I94" s="44"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="41">
         <v>6</v>
       </c>
-      <c r="B95" s="42"/>
+      <c r="B95" s="43"/>
       <c r="C95" s="19" t="s">
         <v>1</v>
       </c>
@@ -5666,9 +5665,9 @@
       <c r="H95" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I95" s="50" t="str">
+      <c r="I95" s="44" t="str">
         <f>IF(H96&gt;H97,B96,B97)</f>
-        <v>Tidak</v>
+        <v>Ya</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -5702,16 +5701,16 @@
         <f>PRODUCT(C96:G96)*$C$50</f>
         <v>6.0877278000000005E-3</v>
       </c>
-      <c r="I96" s="50"/>
+      <c r="I96" s="44"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A97" s="46"/>
+      <c r="A97" s="42"/>
       <c r="B97" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C97" s="24">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D97" s="24">
         <f>K32</f>
@@ -5723,7 +5722,7 @@
       </c>
       <c r="F97" s="24">
         <f>K42</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="G97" s="24">
         <f>K47</f>
@@ -5731,15 +5730,15 @@
       </c>
       <c r="H97" s="20">
         <f>PRODUCT(C97:G97)*$C$51</f>
-        <v>1.2702096000000001E-2</v>
-      </c>
-      <c r="I97" s="50"/>
+        <v>5.1963119999999998E-3</v>
+      </c>
+      <c r="I97" s="44"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="41">
         <v>7</v>
       </c>
-      <c r="B98" s="42"/>
+      <c r="B98" s="43"/>
       <c r="C98" s="19" t="s">
         <v>1</v>
       </c>
@@ -5758,9 +5757,9 @@
       <c r="H98" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I98" s="50" t="str">
+      <c r="I98" s="45" t="str">
         <f>IF(H99&gt;H100,B99,B100)</f>
-        <v>Ya</v>
+        <v>Tidak</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
@@ -5794,16 +5793,16 @@
         <f>PRODUCT(C99:G99)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I99" s="50"/>
+      <c r="I99" s="45"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" s="46"/>
+      <c r="A100" s="42"/>
       <c r="B100" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C100" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D100" s="20">
         <f>K30</f>
@@ -5815,7 +5814,7 @@
       </c>
       <c r="F100" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G100" s="20">
         <f>K46</f>
@@ -5823,15 +5822,15 @@
       </c>
       <c r="H100" s="20">
         <f>PRODUCT(C100:G100)*$C$51</f>
-        <v>6.6686004000000004E-3</v>
-      </c>
-      <c r="I100" s="50"/>
+        <v>3.2736765600000009E-2</v>
+      </c>
+      <c r="I100" s="45"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="41">
         <v>8</v>
       </c>
-      <c r="B101" s="42"/>
+      <c r="B101" s="43"/>
       <c r="C101" s="19" t="s">
         <v>1</v>
       </c>
@@ -5850,7 +5849,7 @@
       <c r="H101" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I101" s="50" t="str">
+      <c r="I101" s="44" t="str">
         <f>IF(H102&gt;H103,B102,B103)</f>
         <v>Ya</v>
       </c>
@@ -5886,16 +5885,16 @@
         <f>PRODUCT(C102:G102)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I102" s="50"/>
+      <c r="I102" s="44"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A103" s="46"/>
+      <c r="A103" s="42"/>
       <c r="B103" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C103" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D103" s="20">
         <f>K30</f>
@@ -5907,7 +5906,7 @@
       </c>
       <c r="F103" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G103" s="20">
         <f>K46</f>
@@ -5915,15 +5914,15 @@
       </c>
       <c r="H103" s="20">
         <f>PRODUCT(C103:G103)*$C$51</f>
-        <v>6.6686003999999997E-4</v>
-      </c>
-      <c r="I103" s="50"/>
+        <v>3.2736765600000005E-3</v>
+      </c>
+      <c r="I103" s="44"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="41">
         <v>9</v>
       </c>
-      <c r="B104" s="42"/>
+      <c r="B104" s="43"/>
       <c r="C104" s="19" t="s">
         <v>0</v>
       </c>
@@ -5942,7 +5941,7 @@
       <c r="H104" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I104" s="50" t="str">
+      <c r="I104" s="44" t="str">
         <f>IF(H105&gt;H106,B105,B106)</f>
         <v>Ya</v>
       </c>
@@ -5978,16 +5977,16 @@
         <f>PRODUCT(C105:G105)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I105" s="50"/>
+      <c r="I105" s="44"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A106" s="46"/>
+      <c r="A106" s="42"/>
       <c r="B106" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C106" s="20">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D106" s="20">
         <f>K31</f>
@@ -5999,7 +5998,7 @@
       </c>
       <c r="F106" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G106" s="20">
         <f>K46</f>
@@ -6007,15 +6006,15 @@
       </c>
       <c r="H106" s="20">
         <f>PRODUCT(C106:G106)*$C$51</f>
-        <v>5.8350253499999999E-4</v>
-      </c>
-      <c r="I106" s="50"/>
+        <v>2.8644669900000008E-3</v>
+      </c>
+      <c r="I106" s="44"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="41">
         <v>10</v>
       </c>
-      <c r="B107" s="42"/>
+      <c r="B107" s="43"/>
       <c r="C107" s="19" t="s">
         <v>1</v>
       </c>
@@ -6034,7 +6033,7 @@
       <c r="H107" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I107" s="50" t="str">
+      <c r="I107" s="44" t="str">
         <f>IF(H108&gt;H109,B108,B109)</f>
         <v>Ya</v>
       </c>
@@ -6070,16 +6069,16 @@
         <f>PRODUCT(C108:G108)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I108" s="50"/>
+      <c r="I108" s="44"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A109" s="46"/>
+      <c r="A109" s="42"/>
       <c r="B109" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C109" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D109" s="20">
         <f>K31</f>
@@ -6091,7 +6090,7 @@
       </c>
       <c r="F109" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G109" s="20">
         <f>K46</f>
@@ -6099,15 +6098,15 @@
       </c>
       <c r="H109" s="20">
         <f>PRODUCT(C109:G109)*$C$51</f>
-        <v>3.3343002000000002E-3</v>
-      </c>
-      <c r="I109" s="50"/>
+        <v>1.6368382800000005E-2</v>
+      </c>
+      <c r="I109" s="44"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="41">
         <v>11</v>
       </c>
-      <c r="B110" s="42"/>
+      <c r="B110" s="43"/>
       <c r="C110" s="19" t="s">
         <v>0</v>
       </c>
@@ -6126,7 +6125,7 @@
       <c r="H110" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I110" s="50" t="str">
+      <c r="I110" s="44" t="str">
         <f>IF(H111&gt;H112,B111,B112)</f>
         <v>Tidak</v>
       </c>
@@ -6162,16 +6161,16 @@
         <f>PRODUCT(C111:G111)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I111" s="50"/>
+      <c r="I111" s="44"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A112" s="46"/>
+      <c r="A112" s="42"/>
       <c r="B112" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C112" s="20">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D112" s="20">
         <f>K30</f>
@@ -6183,7 +6182,7 @@
       </c>
       <c r="F112" s="20">
         <f>K42</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="G112" s="20">
         <f>K47</f>
@@ -6191,15 +6190,15 @@
       </c>
       <c r="H112" s="20">
         <f>PRODUCT(C112:G112)*$C$51</f>
-        <v>6.6686004000000007E-2</v>
-      </c>
-      <c r="I112" s="50"/>
+        <v>2.7280638000000006E-2</v>
+      </c>
+      <c r="I112" s="44"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="41">
         <v>12</v>
       </c>
-      <c r="B113" s="42"/>
+      <c r="B113" s="43"/>
       <c r="C113" s="19" t="s">
         <v>1</v>
       </c>
@@ -6218,7 +6217,7 @@
       <c r="H113" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I113" s="50" t="str">
+      <c r="I113" s="44" t="str">
         <f>IF(H114&gt;H115,B114,B115)</f>
         <v>Tidak</v>
       </c>
@@ -6254,16 +6253,16 @@
         <f>PRODUCT(C114:G114)*$C$50</f>
         <v>6.9574032000000001E-3</v>
       </c>
-      <c r="I114" s="50"/>
+      <c r="I114" s="44"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="46"/>
+      <c r="A115" s="42"/>
       <c r="B115" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C115" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D115" s="20">
         <f>K30</f>
@@ -6275,7 +6274,7 @@
       </c>
       <c r="F115" s="20">
         <f>K42</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="G115" s="20">
         <f>K47</f>
@@ -6283,15 +6282,15 @@
       </c>
       <c r="H115" s="20">
         <f>PRODUCT(C115:G115)*$C$51</f>
-        <v>3.8106288000000002E-2</v>
-      </c>
-      <c r="I115" s="50"/>
+        <v>1.5588936000000003E-2</v>
+      </c>
+      <c r="I115" s="44"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="41">
         <v>13</v>
       </c>
-      <c r="B116" s="42"/>
+      <c r="B116" s="43"/>
       <c r="C116" s="19" t="s">
         <v>0</v>
       </c>
@@ -6310,9 +6309,9 @@
       <c r="H116" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I116" s="49" t="str">
+      <c r="I116" s="44" t="str">
         <f>IF(H117&gt;H118,B117,B118)</f>
-        <v>Ya</v>
+        <v>Tidak</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
@@ -6346,16 +6345,16 @@
         <f>PRODUCT(C117:G117)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I117" s="49"/>
+      <c r="I117" s="44"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="46"/>
+      <c r="A118" s="42"/>
       <c r="B118" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C118" s="20">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D118" s="20">
         <f>K31</f>
@@ -6367,7 +6366,7 @@
       </c>
       <c r="F118" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G118" s="20">
         <f>K47</f>
@@ -6375,15 +6374,15 @@
       </c>
       <c r="H118" s="20">
         <f>PRODUCT(C118:G118)*$C$51</f>
-        <v>3.3343002000000006E-3</v>
-      </c>
-      <c r="I118" s="49"/>
+        <v>1.6368382800000005E-2</v>
+      </c>
+      <c r="I118" s="44"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="41">
         <v>14</v>
       </c>
-      <c r="B119" s="42"/>
+      <c r="B119" s="43"/>
       <c r="C119" s="19" t="s">
         <v>0</v>
       </c>
@@ -6402,7 +6401,7 @@
       <c r="H119" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I119" s="50" t="str">
+      <c r="I119" s="44" t="str">
         <f>IF(H120&gt;H121,B120,B121)</f>
         <v>Tidak</v>
       </c>
@@ -6438,16 +6437,16 @@
         <f>PRODUCT(C120:G120)*$C$50</f>
         <v>9.7403644800000012E-3</v>
       </c>
-      <c r="I120" s="50"/>
+      <c r="I120" s="44"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A121" s="46"/>
+      <c r="A121" s="42"/>
       <c r="B121" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C121" s="20">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D121" s="20">
         <f>K30</f>
@@ -6459,7 +6458,7 @@
       </c>
       <c r="F121" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G121" s="20">
         <f>K46</f>
@@ -6467,15 +6466,15 @@
       </c>
       <c r="H121" s="20">
         <f>PRODUCT(C121:G121)*$C$51</f>
-        <v>1.1670050700000002E-2</v>
-      </c>
-      <c r="I121" s="50"/>
+        <v>5.7289339800000012E-2</v>
+      </c>
+      <c r="I121" s="44"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="41">
         <v>15</v>
       </c>
-      <c r="B122" s="42"/>
+      <c r="B122" s="43"/>
       <c r="C122" s="19" t="s">
         <v>0</v>
       </c>
@@ -6494,7 +6493,7 @@
       <c r="H122" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I122" s="50" t="str">
+      <c r="I122" s="44" t="str">
         <f>IF(H123&gt;H124,B123,B124)</f>
         <v>Tidak</v>
       </c>
@@ -6530,16 +6529,16 @@
         <f>PRODUCT(C123:G123)*$C$50</f>
         <v>2.7829612800000002E-3</v>
       </c>
-      <c r="I123" s="50"/>
+      <c r="I123" s="44"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A124" s="46"/>
+      <c r="A124" s="42"/>
       <c r="B124" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C124" s="20">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D124" s="20">
         <f>K30</f>
@@ -6551,7 +6550,7 @@
       </c>
       <c r="F124" s="20">
         <f>K42</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="G124" s="20">
         <f>K46</f>
@@ -6559,15 +6558,15 @@
       </c>
       <c r="H124" s="20">
         <f>PRODUCT(C124:G124)*$C$51</f>
-        <v>0.11670050700000002</v>
-      </c>
-      <c r="I124" s="50"/>
+        <v>4.7741116500000014E-2</v>
+      </c>
+      <c r="I124" s="44"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="41">
         <v>16</v>
       </c>
-      <c r="B125" s="42"/>
+      <c r="B125" s="43"/>
       <c r="C125" s="19" t="s">
         <v>1</v>
       </c>
@@ -6586,9 +6585,9 @@
       <c r="H125" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I125" s="49" t="str">
+      <c r="I125" s="44" t="str">
         <f>IF(H126&gt;H127,B126,B127)</f>
-        <v>Ya</v>
+        <v>Tidak</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
@@ -6622,16 +6621,16 @@
         <f>PRODUCT(C126:G126)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I126" s="49"/>
+      <c r="I126" s="44"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A127" s="46"/>
+      <c r="A127" s="42"/>
       <c r="B127" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C127" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D127" s="20">
         <f>K30</f>
@@ -6643,7 +6642,7 @@
       </c>
       <c r="F127" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G127" s="20">
         <f>K46</f>
@@ -6651,15 +6650,15 @@
       </c>
       <c r="H127" s="20">
         <f>PRODUCT(C127:G127)*$C$51</f>
-        <v>6.6686004000000004E-3</v>
-      </c>
-      <c r="I127" s="49"/>
+        <v>3.2736765600000009E-2</v>
+      </c>
+      <c r="I127" s="44"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="41">
         <v>17</v>
       </c>
-      <c r="B128" s="42"/>
+      <c r="B128" s="43"/>
       <c r="C128" s="19" t="s">
         <v>1</v>
       </c>
@@ -6678,7 +6677,7 @@
       <c r="H128" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I128" s="50" t="str">
+      <c r="I128" s="44" t="str">
         <f>IF(H129&gt;H130,B129,B130)</f>
         <v>Tidak</v>
       </c>
@@ -6714,16 +6713,16 @@
         <f>PRODUCT(C129:G129)*$C$50</f>
         <v>5.5659225600000004E-3</v>
       </c>
-      <c r="I129" s="50"/>
+      <c r="I129" s="44"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A130" s="46"/>
+      <c r="A130" s="42"/>
       <c r="B130" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C130" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D130" s="20">
         <f>K30</f>
@@ -6735,7 +6734,7 @@
       </c>
       <c r="F130" s="20">
         <f>K42</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="G130" s="20">
         <f>K46</f>
@@ -6743,15 +6742,15 @@
       </c>
       <c r="H130" s="20">
         <f>PRODUCT(C130:G130)*$C$51</f>
-        <v>6.6686004000000007E-2</v>
-      </c>
-      <c r="I130" s="50"/>
+        <v>2.7280638000000006E-2</v>
+      </c>
+      <c r="I130" s="44"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="41">
         <v>18</v>
       </c>
-      <c r="B131" s="42"/>
+      <c r="B131" s="43"/>
       <c r="C131" s="19" t="s">
         <v>0</v>
       </c>
@@ -6770,9 +6769,9 @@
       <c r="H131" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I131" s="49" t="str">
+      <c r="I131" s="44" t="str">
         <f>IF(H132&gt;H133,B132,B133)</f>
-        <v>Ya</v>
+        <v>Tidak</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
@@ -6806,16 +6805,16 @@
         <f>PRODUCT(C132:G132)*$C$50</f>
         <v>9.7403644800000012E-3</v>
       </c>
-      <c r="I132" s="49"/>
+      <c r="I132" s="44"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A133" s="46"/>
+      <c r="A133" s="42"/>
       <c r="B133" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C133" s="20">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D133" s="20">
         <f>K31</f>
@@ -6827,7 +6826,7 @@
       </c>
       <c r="F133" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G133" s="20">
         <f>K46</f>
@@ -6835,9 +6834,9 @@
       </c>
       <c r="H133" s="20">
         <f>PRODUCT(C133:G133)*$C$51</f>
-        <v>5.835025350000001E-3</v>
-      </c>
-      <c r="I133" s="49"/>
+        <v>2.8644669900000006E-2</v>
+      </c>
+      <c r="I133" s="44"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="41">
@@ -6907,7 +6906,7 @@
       </c>
       <c r="C136" s="20">
         <f>K25</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D136" s="20">
         <f>K31</f>
@@ -6919,7 +6918,7 @@
       </c>
       <c r="F136" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G136" s="20">
         <f>K46</f>
@@ -6927,7 +6926,7 @@
       </c>
       <c r="H136" s="20">
         <f>PRODUCT(C136:G136)*$C$51</f>
-        <v>5.8350253499999999E-4</v>
+        <v>2.8644669900000008E-3</v>
       </c>
       <c r="I136" s="40"/>
     </row>
@@ -6935,7 +6934,7 @@
       <c r="A137" s="41">
         <v>20</v>
       </c>
-      <c r="B137" s="42"/>
+      <c r="B137" s="43"/>
       <c r="C137" s="19" t="s">
         <v>1</v>
       </c>
@@ -6954,7 +6953,7 @@
       <c r="H137" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I137" s="43" t="str">
+      <c r="I137" s="46" t="str">
         <f>IF(H138&gt;H139,B138,B139)</f>
         <v>Ya</v>
       </c>
@@ -6990,16 +6989,16 @@
         <f>PRODUCT(C138:G138)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I138" s="44"/>
+      <c r="I138" s="47"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A139" s="46"/>
+      <c r="A139" s="42"/>
       <c r="B139" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C139" s="20">
         <f>K26</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D139" s="20">
         <f>K31</f>
@@ -7011,7 +7010,7 @@
       </c>
       <c r="F139" s="20">
         <f>K41</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G139" s="20">
         <f>K46</f>
@@ -7019,9 +7018,9 @@
       </c>
       <c r="H139" s="20">
         <f>PRODUCT(C139:G139)*$C$51</f>
-        <v>3.3343001999999999E-4</v>
-      </c>
-      <c r="I139" s="45"/>
+        <v>1.6368382800000002E-3</v>
+      </c>
+      <c r="I139" s="48"/>
     </row>
     <row r="153" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -7156,8 +7155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A02A39-F2B8-4A72-BE6A-2B6D7673FEB4}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7763,10 +7762,10 @@
       <c r="H28" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J28" s="47" t="s">
+      <c r="J28" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="K28" s="47"/>
+      <c r="K28" s="49"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="29">
@@ -7793,8 +7792,8 @@
       <c r="H29" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="27">
@@ -7985,7 +7984,7 @@
       <c r="H37" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="50" t="str">
+      <c r="I37" s="44" t="str">
         <f>IF(H38&gt;H39,B38,B39)</f>
         <v>Ya</v>
       </c>
@@ -8021,7 +8020,7 @@
         <f>PRODUCT(C38:G38)*$H$23</f>
         <v>2.3191344000000003E-2</v>
       </c>
-      <c r="I38" s="50"/>
+      <c r="I38" s="44"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="55"/>
@@ -8052,7 +8051,7 @@
         <f>PRODUCT(C39:G39)*$H$24</f>
         <v>3.4642079999999995E-4</v>
       </c>
-      <c r="I39" s="50"/>
+      <c r="I39" s="44"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="62">
@@ -8077,7 +8076,7 @@
       <c r="H40" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I40" s="50" t="str">
+      <c r="I40" s="44" t="str">
         <f>IF(H41&gt;H42,B41,B42)</f>
         <v>Ya</v>
       </c>
@@ -8113,7 +8112,7 @@
         <f>PRODUCT(C41:G41)*$H$23</f>
         <v>1.4494590000000002E-2</v>
       </c>
-      <c r="I41" s="50"/>
+      <c r="I41" s="44"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="55"/>
@@ -8144,7 +8143,7 @@
         <f>PRODUCT(C42:G42)*$H$24</f>
         <v>6.9284159999999991E-4</v>
       </c>
-      <c r="I42" s="50"/>
+      <c r="I42" s="44"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="62">
@@ -8169,7 +8168,7 @@
       <c r="H43" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I43" s="50" t="str">
+      <c r="I43" s="44" t="str">
         <f>IF(H44&gt;H45,B44,B45)</f>
         <v>Ya</v>
       </c>
@@ -8205,7 +8204,7 @@
         <f>PRODUCT(C44:G44)*$H$23</f>
         <v>4.6382688000000004E-3</v>
       </c>
-      <c r="I44" s="50"/>
+      <c r="I44" s="44"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="55"/>
@@ -8236,7 +8235,7 @@
         <f>PRODUCT(C45:G45)*$H$24</f>
         <v>2.3094719999999999E-3</v>
       </c>
-      <c r="I45" s="50"/>
+      <c r="I45" s="44"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="62">
@@ -8261,7 +8260,7 @@
       <c r="H46" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I46" s="49" t="str">
+      <c r="I46" s="45" t="str">
         <f>IF(H47&gt;H48,B47,B48)</f>
         <v>Ya</v>
       </c>
@@ -8297,7 +8296,7 @@
         <f>PRODUCT(C47:G47)*$H$23</f>
         <v>2.3191344000000003E-2</v>
       </c>
-      <c r="I47" s="49"/>
+      <c r="I47" s="45"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="55"/>
@@ -8328,7 +8327,7 @@
         <f>PRODUCT(C48:G48)*$H$24</f>
         <v>3.4642079999999995E-4</v>
       </c>
-      <c r="I48" s="49"/>
+      <c r="I48" s="45"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="62">
@@ -8353,7 +8352,7 @@
       <c r="H49" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I49" s="50" t="str">
+      <c r="I49" s="44" t="str">
         <f>IF(H50&gt;H51,B50,B51)</f>
         <v>Tidak</v>
       </c>
@@ -8389,7 +8388,7 @@
         <f>PRODUCT(C50:G50)*$H$23</f>
         <v>2.3191344000000002E-3</v>
       </c>
-      <c r="I50" s="50"/>
+      <c r="I50" s="44"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="55"/>
@@ -8420,7 +8419,7 @@
         <f>PRODUCT(C51:G51)*$H$24</f>
         <v>4.0415759999999998E-3</v>
       </c>
-      <c r="I51" s="50"/>
+      <c r="I51" s="44"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="62">
@@ -8445,7 +8444,7 @@
       <c r="H52" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I52" s="50" t="str">
+      <c r="I52" s="44" t="str">
         <f>IF(H53&gt;H54,B53,B54)</f>
         <v>Tidak</v>
       </c>
@@ -8481,7 +8480,7 @@
         <f>PRODUCT(C53:G53)*$H$23</f>
         <v>1.6565245714285713E-3</v>
       </c>
-      <c r="I53" s="50"/>
+      <c r="I53" s="44"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="55"/>
@@ -8512,7 +8511,7 @@
         <f>PRODUCT(C54:G54)*$H$24</f>
         <v>1.3196982857142856E-2</v>
       </c>
-      <c r="I54" s="50"/>
+      <c r="I54" s="44"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="62">
@@ -8537,7 +8536,7 @@
       <c r="H55" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I55" s="50" t="str">
+      <c r="I55" s="44" t="str">
         <f>IF(H56&gt;H57,B56,B57)</f>
         <v>Tidak</v>
       </c>
@@ -8573,7 +8572,7 @@
         <f>PRODUCT(C56:G56)*$H$23</f>
         <v>2.6504393142857143E-3</v>
       </c>
-      <c r="I56" s="50"/>
+      <c r="I56" s="44"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="55"/>
@@ -8604,10 +8603,14 @@
         <f>PRODUCT(C57:G57)*$H$24</f>
         <v>0.12124728000000001</v>
       </c>
-      <c r="I57" s="50"/>
+      <c r="I57" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:B12"/>
     <mergeCell ref="A13:A14"/>
@@ -8615,16 +8618,12 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="F17:G18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A22:B23"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="I55:I57"/>
     <mergeCell ref="A56:A57"/>

</xml_diff>

<commit_message>
SHOW: show all probability percentage in table data
</commit_message>
<xml_diff>
--- a/uploads/dataset.xlsx
+++ b/uploads/dataset.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iqbal al-ayyubi\Documents\upn-jatim\semester 3\Statkom\Review Jurnal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iqbal al-ayyubi\Documents\upn-jatim\semester 3\Statkom\naive-bayes-app\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625848C1-B3E8-40E3-A8FF-4AD2079F6C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816D083E-D369-4EAC-A14D-F45EACA6BB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATASET" sheetId="1" r:id="rId1"/>
     <sheet name="TRAINING TESTING" sheetId="2" r:id="rId2"/>
-    <sheet name="TESTING" sheetId="3" r:id="rId3"/>
+    <sheet name="DATA_APP" sheetId="4" r:id="rId3"/>
+    <sheet name="TESTING" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="44">
   <si>
     <t>Wanita</t>
   </si>
@@ -526,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -869,6 +870,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -914,7 +926,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1017,60 +1029,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="23" xfId="25" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="16" xfId="23" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="24" xfId="25" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="23" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="22" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="24" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="28" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1092,17 +1050,59 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="15" xfId="24" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="23" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="19" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="28" xfId="23" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="28" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="24" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="23" xfId="25" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="24" xfId="25" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="16" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="22" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="24" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="10" xfId="22" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1111,6 +1111,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="10" xfId="30" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="24" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="28" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1158,7 +1179,295 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="65">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1685,95 +1994,111 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H28" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H28" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <autoFilter ref="A1:H28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H28">
     <sortCondition descending="1" ref="H1:H28"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="A1" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A2" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="A3" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="A1" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="A2" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="A3" dataDxfId="60">
       <calculatedColumnFormula array="1">_xlfn.IFS(AND(Table1[[#This Row],[A2]]&gt;=$D$32,Table1[[#This Row],[A2]]&lt;$E$32),$F$32,AND(Table1[[#This Row],[A2]]&gt;=$D$33,Table1[[#This Row],[A2]]&lt;$E$33),$F$33,AND(Table1[[#This Row],[A2]]&gt;=$D$34,Table1[[#This Row],[A2]]&lt;=$E$34),$F$34)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="A4" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="A5" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="A6" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{A4FBB985-02F1-4466-AEE2-AB9CC6AD12C1}" name="A7" dataDxfId="44">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="A4" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="A5" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="A6" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{A4FBB985-02F1-4466-AEE2-AB9CC6AD12C1}" name="A7" dataDxfId="56">
       <calculatedColumnFormula array="1">_xlfn.IFS(AND(Table1[[#This Row],[A6]]&gt;=$D$39,Table1[[#This Row],[A6]]&lt;$E$39),$F$39,AND(Table1[[#This Row],[A6]]&gt;=$D$40,Table1[[#This Row],[A6]]&lt;=$E$40),$F$40)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Kelas" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Kelas" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C986878F-8EE5-43A4-8F1E-B09A11DB2EF5}" name="Table5" displayName="Table5" ref="A56:H76" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C986878F-8EE5-43A4-8F1E-B09A11DB2EF5}" name="Table5" displayName="Table5" ref="A56:H76" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A56:H76" xr:uid="{C986878F-8EE5-43A4-8F1E-B09A11DB2EF5}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5EB608ED-5A77-447B-8FD2-A9CCB68A82F8}" name="No" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{83540509-4260-4FA0-A6F8-F41A7F0A1B92}" name="A1" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{A1BF85CE-3F21-4A8D-8FD6-2511C4E8253B}" name="A3" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{1D4237E5-26CE-45EF-B359-DAC17B31C28E}" name="A4" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{10C96685-023E-40D9-942D-C36681C12ED8}" name="A5" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{9EEE3C16-42E5-4F47-A7BF-D49ADFA50BC1}" name="A7" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{A249E022-445E-4F81-8DEB-63698942B392}" name="Kelas Asli" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{C6CD83B8-07DA-474F-802B-76045229FC10}" name="Prediction" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{5EB608ED-5A77-447B-8FD2-A9CCB68A82F8}" name="No" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{83540509-4260-4FA0-A6F8-F41A7F0A1B92}" name="A1" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{A1BF85CE-3F21-4A8D-8FD6-2511C4E8253B}" name="A3" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{1D4237E5-26CE-45EF-B359-DAC17B31C28E}" name="A4" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{10C96685-023E-40D9-942D-C36681C12ED8}" name="A5" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{9EEE3C16-42E5-4F47-A7BF-D49ADFA50BC1}" name="A7" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{A249E022-445E-4F81-8DEB-63698942B392}" name="Kelas Asli" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{C6CD83B8-07DA-474F-802B-76045229FC10}" name="Prediction" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50333CBC-2500-4142-92CF-881F50BF3F23}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50333CBC-2500-4142-92CF-881F50BF3F23}" name="Table2" displayName="Table2" ref="A1:H21" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A1:H21" xr:uid="{50333CBC-2500-4142-92CF-881F50BF3F23}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H21">
     <sortCondition descending="1" ref="H1:H21"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F9556ADE-413E-4812-94B2-2CEBBB30EEB2}" name="A1" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{9BF2FAE3-B5A9-469F-907E-3D7278E1D10C}" name="A2" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{10B99B09-D0F5-4B8C-9FCB-0C5077497766}" name="A3" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{92400868-0B20-4BA9-9E36-E1B024036CC3}" name="A4" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{9C482C5D-0C4E-475D-9F16-887EA23CCF49}" name="A5" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{BD85F050-D362-499F-BA0E-2CC9F710201F}" name="A6" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{3E37FF79-B776-40FF-83D9-B2C26CCBB558}" name="A7" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{0279EC89-3A08-4B27-9040-EAB5E246648C}" name="Kelas" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{F9556ADE-413E-4812-94B2-2CEBBB30EEB2}" name="A1" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{9BF2FAE3-B5A9-469F-907E-3D7278E1D10C}" name="A2" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{10B99B09-D0F5-4B8C-9FCB-0C5077497766}" name="A3" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{92400868-0B20-4BA9-9E36-E1B024036CC3}" name="A4" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{9C482C5D-0C4E-475D-9F16-887EA23CCF49}" name="A5" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{BD85F050-D362-499F-BA0E-2CC9F710201F}" name="A6" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{3E37FF79-B776-40FF-83D9-B2C26CCBB558}" name="A7" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{0279EC89-3A08-4B27-9040-EAB5E246648C}" name="Kelas" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E43C5A67-0B0E-4FC9-88BC-F5BCF9409F37}" name="Table3" displayName="Table3" ref="A1:H8" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
-  <autoFilter ref="A1:H8" xr:uid="{E43C5A67-0B0E-4FC9-88BC-F5BCF9409F37}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D57249E6-A2DD-443B-96EF-7E2A50FE96EE}" name="A1" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{210CD1B4-4A40-48CB-BE25-18CAB49D43C2}" name="A2" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{3312FDAA-8C88-44BB-88D5-B188BDC0F26D}" name="A3" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{5995CFA6-6AD2-4936-998F-2AA16B2B3EA1}" name="A4" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{092C32B2-067B-476E-A4D3-2F7762D153C1}" name="A5" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{042C6AC1-6CCA-4920-85E5-614E885036FF}" name="A6" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{ECE2C959-8E6A-4733-A47E-8F83388B4903}" name="A7" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{C9EA31FF-440C-4B76-823B-CCAB36E71730}" name="Kelas" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3B840F97-9D3E-4002-8C65-50C00E9E68B6}" name="Table4" displayName="Table4" ref="A1:G21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:G21" xr:uid="{3B840F97-9D3E-4002-8C65-50C00E9E68B6}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{EBDB54CD-4136-44A2-A5D8-16D6A7FDFEF6}" name="No" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{A51E0D62-F7AE-4CF5-AB71-B0970ED0A5C1}" name="A1" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{28AEF9E7-B4DC-4C35-B9B1-42FB8D0CD93F}" name="A3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{821674A5-3142-4BB7-A3D6-3009C13EBE3F}" name="A4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{4C341E52-534C-4DA0-9857-2E54F276D560}" name="A5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{7994CE9D-28B4-410B-95AA-5D1276DC5454}" name="A7" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{862BF86E-35D0-41F0-8FA0-FE9EC6C5BA15}" name="Kelas" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A14F7FD6-DC4E-4509-A422-2947C1FD40F1}" name="Table8" displayName="Table8" ref="A27:H34" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E43C5A67-0B0E-4FC9-88BC-F5BCF9409F37}" name="Table3" displayName="Table3" ref="A1:H8" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
+  <autoFilter ref="A1:H8" xr:uid="{E43C5A67-0B0E-4FC9-88BC-F5BCF9409F37}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D57249E6-A2DD-443B-96EF-7E2A50FE96EE}" name="A1" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{210CD1B4-4A40-48CB-BE25-18CAB49D43C2}" name="A2" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{3312FDAA-8C88-44BB-88D5-B188BDC0F26D}" name="A3" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{5995CFA6-6AD2-4936-998F-2AA16B2B3EA1}" name="A4" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{092C32B2-067B-476E-A4D3-2F7762D153C1}" name="A5" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{042C6AC1-6CCA-4920-85E5-614E885036FF}" name="A6" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{ECE2C959-8E6A-4733-A47E-8F83388B4903}" name="A7" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{C9EA31FF-440C-4B76-823B-CCAB36E71730}" name="Kelas" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A14F7FD6-DC4E-4509-A422-2947C1FD40F1}" name="Table8" displayName="Table8" ref="A27:H34" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A27:H34" xr:uid="{A14F7FD6-DC4E-4509-A422-2947C1FD40F1}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{44CE8644-5295-432D-8B3F-EE68F19519DB}" name="No" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{32A7D7FA-4120-46AA-9921-71C36BFB5E4F}" name="A1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E43E2477-B25B-4F31-8D78-B5E79037476A}" name="A3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{321D3E0C-2282-4D82-A4BA-A11F380E5562}" name="A4" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{019591A9-F012-4A73-BA2D-DEBC506C80F8}" name="A5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{6403F498-3368-417E-9BB5-030E5CA84CF0}" name="A7" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{CC3D58F9-0B78-424C-8483-09CBB1789DB2}" name="Kelas" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{6BFBC307-003C-422A-AAFC-F1B43CD635DC}" name="Prediction" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{44CE8644-5295-432D-8B3F-EE68F19519DB}" name="No" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{32A7D7FA-4120-46AA-9921-71C36BFB5E4F}" name="A1" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{E43E2477-B25B-4F31-8D78-B5E79037476A}" name="A3" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{321D3E0C-2282-4D82-A4BA-A11F380E5562}" name="A4" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{019591A9-F012-4A73-BA2D-DEBC506C80F8}" name="A5" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{6403F498-3368-417E-9BB5-030E5CA84CF0}" name="A7" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{CC3D58F9-0B78-424C-8483-09CBB1789DB2}" name="Kelas" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{6BFBC307-003C-422A-AAFC-F1B43CD635DC}" name="Prediction" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3210,8 +3535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D884DC29-9C63-4ED2-98E5-F89FE5DACB23}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95:I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3829,29 +4154,29 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="52" t="s">
+      <c r="B23" s="44"/>
+      <c r="C23" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="52"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="53" t="s">
+      <c r="F23" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="53"/>
-      <c r="H23" s="36" t="s">
+      <c r="G23" s="46"/>
+      <c r="H23" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="38"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="49"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="51"/>
-      <c r="B24" s="51"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="13" t="s">
         <v>3</v>
       </c>
@@ -3859,8 +4184,8 @@
         <v>2</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
       <c r="H24" s="13" t="s">
         <v>3</v>
       </c>
@@ -3954,29 +4279,29 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="52" t="s">
+      <c r="B28" s="44"/>
+      <c r="C28" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="52"/>
+      <c r="D28" s="45"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="53" t="s">
+      <c r="F28" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="53"/>
-      <c r="H28" s="36" t="s">
+      <c r="G28" s="46"/>
+      <c r="H28" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="38"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="49"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="51"/>
-      <c r="B29" s="51"/>
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
       <c r="C29" s="13" t="s">
         <v>3</v>
       </c>
@@ -3984,8 +4309,8 @@
         <v>2</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
       <c r="H29" s="13" t="s">
         <v>3</v>
       </c>
@@ -4114,29 +4439,29 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="52" t="s">
+      <c r="B34" s="44"/>
+      <c r="C34" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="52"/>
+      <c r="D34" s="45"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="53" t="s">
+      <c r="F34" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="53"/>
-      <c r="H34" s="36" t="s">
+      <c r="G34" s="46"/>
+      <c r="H34" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="38"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="49"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="51"/>
-      <c r="B35" s="51"/>
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
       <c r="C35" s="13" t="s">
         <v>3</v>
       </c>
@@ -4144,8 +4469,8 @@
         <v>2</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
       <c r="H35" s="13" t="s">
         <v>3</v>
       </c>
@@ -4239,29 +4564,29 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="51"/>
-      <c r="C39" s="52" t="s">
+      <c r="B39" s="44"/>
+      <c r="C39" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="52"/>
+      <c r="D39" s="45"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="53" t="s">
+      <c r="F39" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="53"/>
-      <c r="H39" s="36" t="s">
+      <c r="G39" s="46"/>
+      <c r="H39" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="38"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="49"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="51"/>
-      <c r="B40" s="51"/>
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
       <c r="C40" s="13" t="s">
         <v>3</v>
       </c>
@@ -4269,8 +4594,8 @@
         <v>2</v>
       </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
       <c r="H40" s="13" t="s">
         <v>3</v>
       </c>
@@ -4364,29 +4689,29 @@
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="52" t="s">
+      <c r="B44" s="44"/>
+      <c r="C44" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="52"/>
+      <c r="D44" s="45"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="53" t="s">
+      <c r="F44" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="G44" s="53"/>
-      <c r="H44" s="36" t="s">
+      <c r="G44" s="46"/>
+      <c r="H44" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="38"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="49"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="51"/>
-      <c r="B45" s="51"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
       <c r="C45" s="13" t="s">
         <v>3</v>
       </c>
@@ -4394,8 +4719,8 @@
         <v>2</v>
       </c>
       <c r="E45" s="1"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
       <c r="H45" s="13" t="s">
         <v>3</v>
       </c>
@@ -4481,11 +4806,11 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
-      <c r="B49" s="59" t="s">
+      <c r="B49" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
@@ -4531,16 +4856,16 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="57"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="57"/>
-      <c r="H55" s="58"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="40"/>
       <c r="J55" s="35" t="s">
         <v>16</v>
       </c>
@@ -4600,8 +4925,8 @@
       <c r="G57" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H57" s="7" t="s">
-        <v>3</v>
+      <c r="H57" s="25" t="s">
+        <v>2</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>18</v>
@@ -4905,10 +5230,10 @@
       <c r="H67" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J67" s="49" t="s">
+      <c r="J67" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="K67" s="49"/>
+      <c r="K67" s="58"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="7">
@@ -4935,8 +5260,8 @@
       <c r="H68" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J68" s="49"/>
-      <c r="K68" s="49"/>
+      <c r="J68" s="58"/>
+      <c r="K68" s="58"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="7">
@@ -4963,11 +5288,11 @@
       <c r="H69" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J69" s="50">
+      <c r="J69" s="59">
         <f>17/20*100</f>
         <v>85</v>
       </c>
-      <c r="K69" s="50"/>
+      <c r="K69" s="59"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="7">
@@ -4994,8 +5319,8 @@
       <c r="H70" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J70" s="50"/>
-      <c r="K70" s="50"/>
+      <c r="J70" s="59"/>
+      <c r="K70" s="59"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="7">
@@ -5022,8 +5347,8 @@
       <c r="H71" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J71" s="50"/>
-      <c r="K71" s="50"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="59"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="7">
@@ -5050,8 +5375,8 @@
       <c r="H72" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J72" s="50"/>
-      <c r="K72" s="50"/>
+      <c r="J72" s="59"/>
+      <c r="K72" s="59"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="7">
@@ -5158,10 +5483,10 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79" s="54">
+      <c r="A79" s="36">
         <v>1</v>
       </c>
-      <c r="B79" s="54"/>
+      <c r="B79" s="36"/>
       <c r="C79" s="22" t="s">
         <v>17</v>
       </c>
@@ -5185,8 +5510,8 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A80" s="54"/>
-      <c r="B80" s="54"/>
+      <c r="A80" s="36"/>
+      <c r="B80" s="36"/>
       <c r="C80" s="23" t="s">
         <v>0</v>
       </c>
@@ -5205,13 +5530,13 @@
       <c r="H80" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="45" t="str">
+      <c r="I80" s="43" t="str">
         <f>IF(H81&gt;H82,B81,B82)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="55" t="s">
+      <c r="A81" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B81" s="14" t="s">
@@ -5241,10 +5566,10 @@
         <f>PRODUCT(C81:G81)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I81" s="45"/>
+      <c r="I81" s="43"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="55"/>
+      <c r="A82" s="37"/>
       <c r="B82" s="14" t="s">
         <v>2</v>
       </c>
@@ -5272,13 +5597,13 @@
         <f>PRODUCT(C82:G82)*$C$51</f>
         <v>3.2736765600000009E-2</v>
       </c>
-      <c r="I82" s="45"/>
+      <c r="I82" s="43"/>
     </row>
     <row r="83" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="41">
-        <v>2</v>
-      </c>
-      <c r="B83" s="43"/>
+      <c r="A83" s="53">
+        <v>2</v>
+      </c>
+      <c r="B83" s="54"/>
       <c r="C83" s="19" t="s">
         <v>1</v>
       </c>
@@ -5297,13 +5622,13 @@
       <c r="H83" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I83" s="44" t="str">
+      <c r="I83" s="52" t="str">
         <f>IF(H84&gt;H85,B84,B85)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84" s="39" t="s">
+      <c r="A84" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B84" s="14" t="s">
@@ -5333,10 +5658,10 @@
         <f>PRODUCT(C84:G84)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I84" s="44"/>
+      <c r="I84" s="52"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" s="42"/>
+      <c r="A85" s="51"/>
       <c r="B85" s="14" t="s">
         <v>2</v>
       </c>
@@ -5364,13 +5689,13 @@
         <f>PRODUCT(C85:G85)*$C$51</f>
         <v>1.8706723200000004E-2</v>
       </c>
-      <c r="I85" s="44"/>
+      <c r="I85" s="52"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86" s="41">
-        <v>3</v>
-      </c>
-      <c r="B86" s="43"/>
+      <c r="A86" s="53">
+        <v>3</v>
+      </c>
+      <c r="B86" s="54"/>
       <c r="C86" s="19" t="s">
         <v>1</v>
       </c>
@@ -5389,13 +5714,13 @@
       <c r="H86" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I86" s="44" t="str">
+      <c r="I86" s="52" t="str">
         <f>IF(H87&gt;H88,B87,B88)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87" s="39" t="s">
+      <c r="A87" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B87" s="14" t="s">
@@ -5425,10 +5750,10 @@
         <f>PRODUCT(C87:G87)*$C$50</f>
         <v>3.0438639000000003E-2</v>
       </c>
-      <c r="I87" s="44"/>
+      <c r="I87" s="52"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="42"/>
+      <c r="A88" s="51"/>
       <c r="B88" s="14" t="s">
         <v>2</v>
       </c>
@@ -5456,13 +5781,13 @@
         <f>PRODUCT(C88:G88)*$C$51</f>
         <v>9.3533616000000016E-4</v>
       </c>
-      <c r="I88" s="44"/>
+      <c r="I88" s="52"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A89" s="41">
+      <c r="A89" s="53">
         <v>4</v>
       </c>
-      <c r="B89" s="43"/>
+      <c r="B89" s="54"/>
       <c r="C89" s="19" t="s">
         <v>0</v>
       </c>
@@ -5481,13 +5806,13 @@
       <c r="H89" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I89" s="44" t="str">
+      <c r="I89" s="43" t="str">
         <f>IF(H90&gt;H91,B90,B91)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A90" s="39" t="s">
+      <c r="A90" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B90" s="14" t="s">
@@ -5517,10 +5842,10 @@
         <f>PRODUCT(C90:G90)*$C$50</f>
         <v>2.4350911200000003E-3</v>
       </c>
-      <c r="I90" s="44"/>
+      <c r="I90" s="43"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91" s="42"/>
+      <c r="A91" s="51"/>
       <c r="B91" s="14" t="s">
         <v>2</v>
       </c>
@@ -5548,13 +5873,13 @@
         <f>PRODUCT(C91:G91)*$C$51</f>
         <v>1.9096446600000004E-2</v>
       </c>
-      <c r="I91" s="44"/>
+      <c r="I91" s="43"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92" s="41">
+      <c r="A92" s="53">
         <v>5</v>
       </c>
-      <c r="B92" s="43"/>
+      <c r="B92" s="54"/>
       <c r="C92" s="19" t="s">
         <v>0</v>
       </c>
@@ -5573,13 +5898,13 @@
       <c r="H92" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I92" s="44" t="str">
+      <c r="I92" s="52" t="str">
         <f>IF(H93&gt;H94,B93,B94)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" s="39" t="s">
+      <c r="A93" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B93" s="14" t="s">
@@ -5609,10 +5934,10 @@
         <f>PRODUCT(C93:G93)*$C$50</f>
         <v>3.8048298750000004E-3</v>
       </c>
-      <c r="I93" s="44"/>
+      <c r="I93" s="52"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94" s="42"/>
+      <c r="A94" s="51"/>
       <c r="B94" s="14" t="s">
         <v>2</v>
       </c>
@@ -5640,13 +5965,13 @@
         <f>PRODUCT(C94:G94)*$C$51</f>
         <v>9.0935460000000001E-4</v>
       </c>
-      <c r="I94" s="44"/>
+      <c r="I94" s="52"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A95" s="41">
+      <c r="A95" s="53">
         <v>6</v>
       </c>
-      <c r="B95" s="43"/>
+      <c r="B95" s="54"/>
       <c r="C95" s="19" t="s">
         <v>1</v>
       </c>
@@ -5665,13 +5990,13 @@
       <c r="H95" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I95" s="44" t="str">
+      <c r="I95" s="52" t="str">
         <f>IF(H96&gt;H97,B96,B97)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" s="39" t="s">
+      <c r="A96" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B96" s="14" t="s">
@@ -5701,10 +6026,10 @@
         <f>PRODUCT(C96:G96)*$C$50</f>
         <v>6.0877278000000005E-3</v>
       </c>
-      <c r="I96" s="44"/>
+      <c r="I96" s="52"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A97" s="42"/>
+      <c r="A97" s="51"/>
       <c r="B97" s="14" t="s">
         <v>2</v>
       </c>
@@ -5732,13 +6057,13 @@
         <f>PRODUCT(C97:G97)*$C$51</f>
         <v>5.1963119999999998E-3</v>
       </c>
-      <c r="I97" s="44"/>
+      <c r="I97" s="52"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A98" s="41">
+      <c r="A98" s="53">
         <v>7</v>
       </c>
-      <c r="B98" s="43"/>
+      <c r="B98" s="54"/>
       <c r="C98" s="19" t="s">
         <v>1</v>
       </c>
@@ -5757,13 +6082,13 @@
       <c r="H98" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I98" s="45" t="str">
+      <c r="I98" s="43" t="str">
         <f>IF(H99&gt;H100,B99,B100)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" s="39" t="s">
+      <c r="A99" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B99" s="14" t="s">
@@ -5793,10 +6118,10 @@
         <f>PRODUCT(C99:G99)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I99" s="45"/>
+      <c r="I99" s="43"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" s="42"/>
+      <c r="A100" s="51"/>
       <c r="B100" s="14" t="s">
         <v>2</v>
       </c>
@@ -5824,13 +6149,13 @@
         <f>PRODUCT(C100:G100)*$C$51</f>
         <v>3.2736765600000009E-2</v>
       </c>
-      <c r="I100" s="45"/>
+      <c r="I100" s="43"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A101" s="41">
+      <c r="A101" s="53">
         <v>8</v>
       </c>
-      <c r="B101" s="43"/>
+      <c r="B101" s="54"/>
       <c r="C101" s="19" t="s">
         <v>1</v>
       </c>
@@ -5849,13 +6174,13 @@
       <c r="H101" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I101" s="44" t="str">
+      <c r="I101" s="52" t="str">
         <f>IF(H102&gt;H103,B102,B103)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A102" s="39" t="s">
+      <c r="A102" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B102" s="14" t="s">
@@ -5885,10 +6210,10 @@
         <f>PRODUCT(C102:G102)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I102" s="44"/>
+      <c r="I102" s="52"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A103" s="42"/>
+      <c r="A103" s="51"/>
       <c r="B103" s="14" t="s">
         <v>2</v>
       </c>
@@ -5916,13 +6241,13 @@
         <f>PRODUCT(C103:G103)*$C$51</f>
         <v>3.2736765600000005E-3</v>
       </c>
-      <c r="I103" s="44"/>
+      <c r="I103" s="52"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A104" s="41">
+      <c r="A104" s="53">
         <v>9</v>
       </c>
-      <c r="B104" s="43"/>
+      <c r="B104" s="54"/>
       <c r="C104" s="19" t="s">
         <v>0</v>
       </c>
@@ -5941,13 +6266,13 @@
       <c r="H104" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I104" s="44" t="str">
+      <c r="I104" s="52" t="str">
         <f>IF(H105&gt;H106,B105,B106)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A105" s="39" t="s">
+      <c r="A105" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B105" s="14" t="s">
@@ -5977,10 +6302,10 @@
         <f>PRODUCT(C105:G105)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I105" s="44"/>
+      <c r="I105" s="52"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A106" s="42"/>
+      <c r="A106" s="51"/>
       <c r="B106" s="14" t="s">
         <v>2</v>
       </c>
@@ -6008,13 +6333,13 @@
         <f>PRODUCT(C106:G106)*$C$51</f>
         <v>2.8644669900000008E-3</v>
       </c>
-      <c r="I106" s="44"/>
+      <c r="I106" s="52"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A107" s="41">
+      <c r="A107" s="53">
         <v>10</v>
       </c>
-      <c r="B107" s="43"/>
+      <c r="B107" s="54"/>
       <c r="C107" s="19" t="s">
         <v>1</v>
       </c>
@@ -6033,13 +6358,13 @@
       <c r="H107" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I107" s="44" t="str">
+      <c r="I107" s="52" t="str">
         <f>IF(H108&gt;H109,B108,B109)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A108" s="39" t="s">
+      <c r="A108" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B108" s="14" t="s">
@@ -6069,10 +6394,10 @@
         <f>PRODUCT(C108:G108)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I108" s="44"/>
+      <c r="I108" s="52"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A109" s="42"/>
+      <c r="A109" s="51"/>
       <c r="B109" s="14" t="s">
         <v>2</v>
       </c>
@@ -6100,13 +6425,13 @@
         <f>PRODUCT(C109:G109)*$C$51</f>
         <v>1.6368382800000005E-2</v>
       </c>
-      <c r="I109" s="44"/>
+      <c r="I109" s="52"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A110" s="41">
+      <c r="A110" s="53">
         <v>11</v>
       </c>
-      <c r="B110" s="43"/>
+      <c r="B110" s="54"/>
       <c r="C110" s="19" t="s">
         <v>0</v>
       </c>
@@ -6125,13 +6450,13 @@
       <c r="H110" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I110" s="44" t="str">
+      <c r="I110" s="52" t="str">
         <f>IF(H111&gt;H112,B111,B112)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A111" s="39" t="s">
+      <c r="A111" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B111" s="14" t="s">
@@ -6161,10 +6486,10 @@
         <f>PRODUCT(C111:G111)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I111" s="44"/>
+      <c r="I111" s="52"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A112" s="42"/>
+      <c r="A112" s="51"/>
       <c r="B112" s="14" t="s">
         <v>2</v>
       </c>
@@ -6192,13 +6517,13 @@
         <f>PRODUCT(C112:G112)*$C$51</f>
         <v>2.7280638000000006E-2</v>
       </c>
-      <c r="I112" s="44"/>
+      <c r="I112" s="52"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113" s="41">
+      <c r="A113" s="53">
         <v>12</v>
       </c>
-      <c r="B113" s="43"/>
+      <c r="B113" s="54"/>
       <c r="C113" s="19" t="s">
         <v>1</v>
       </c>
@@ -6217,13 +6542,13 @@
       <c r="H113" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I113" s="44" t="str">
+      <c r="I113" s="52" t="str">
         <f>IF(H114&gt;H115,B114,B115)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114" s="39" t="s">
+      <c r="A114" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B114" s="14" t="s">
@@ -6253,10 +6578,10 @@
         <f>PRODUCT(C114:G114)*$C$50</f>
         <v>6.9574032000000001E-3</v>
       </c>
-      <c r="I114" s="44"/>
+      <c r="I114" s="52"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="42"/>
+      <c r="A115" s="51"/>
       <c r="B115" s="14" t="s">
         <v>2</v>
       </c>
@@ -6284,13 +6609,13 @@
         <f>PRODUCT(C115:G115)*$C$51</f>
         <v>1.5588936000000003E-2</v>
       </c>
-      <c r="I115" s="44"/>
+      <c r="I115" s="52"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="41">
+      <c r="A116" s="53">
         <v>13</v>
       </c>
-      <c r="B116" s="43"/>
+      <c r="B116" s="54"/>
       <c r="C116" s="19" t="s">
         <v>0</v>
       </c>
@@ -6309,13 +6634,13 @@
       <c r="H116" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I116" s="44" t="str">
+      <c r="I116" s="52" t="str">
         <f>IF(H117&gt;H118,B117,B118)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117" s="39" t="s">
+      <c r="A117" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B117" s="14" t="s">
@@ -6345,10 +6670,10 @@
         <f>PRODUCT(C117:G117)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I117" s="44"/>
+      <c r="I117" s="52"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="42"/>
+      <c r="A118" s="51"/>
       <c r="B118" s="14" t="s">
         <v>2</v>
       </c>
@@ -6376,13 +6701,13 @@
         <f>PRODUCT(C118:G118)*$C$51</f>
         <v>1.6368382800000005E-2</v>
       </c>
-      <c r="I118" s="44"/>
+      <c r="I118" s="52"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119" s="41">
+      <c r="A119" s="53">
         <v>14</v>
       </c>
-      <c r="B119" s="43"/>
+      <c r="B119" s="54"/>
       <c r="C119" s="19" t="s">
         <v>0</v>
       </c>
@@ -6401,13 +6726,13 @@
       <c r="H119" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I119" s="44" t="str">
+      <c r="I119" s="52" t="str">
         <f>IF(H120&gt;H121,B120,B121)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A120" s="39" t="s">
+      <c r="A120" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B120" s="14" t="s">
@@ -6437,10 +6762,10 @@
         <f>PRODUCT(C120:G120)*$C$50</f>
         <v>9.7403644800000012E-3</v>
       </c>
-      <c r="I120" s="44"/>
+      <c r="I120" s="52"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A121" s="42"/>
+      <c r="A121" s="51"/>
       <c r="B121" s="14" t="s">
         <v>2</v>
       </c>
@@ -6468,13 +6793,13 @@
         <f>PRODUCT(C121:G121)*$C$51</f>
         <v>5.7289339800000012E-2</v>
       </c>
-      <c r="I121" s="44"/>
+      <c r="I121" s="52"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A122" s="41">
+      <c r="A122" s="53">
         <v>15</v>
       </c>
-      <c r="B122" s="43"/>
+      <c r="B122" s="54"/>
       <c r="C122" s="19" t="s">
         <v>0</v>
       </c>
@@ -6493,13 +6818,13 @@
       <c r="H122" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I122" s="44" t="str">
+      <c r="I122" s="52" t="str">
         <f>IF(H123&gt;H124,B123,B124)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A123" s="39" t="s">
+      <c r="A123" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B123" s="14" t="s">
@@ -6529,10 +6854,10 @@
         <f>PRODUCT(C123:G123)*$C$50</f>
         <v>2.7829612800000002E-3</v>
       </c>
-      <c r="I123" s="44"/>
+      <c r="I123" s="52"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A124" s="42"/>
+      <c r="A124" s="51"/>
       <c r="B124" s="14" t="s">
         <v>2</v>
       </c>
@@ -6560,13 +6885,13 @@
         <f>PRODUCT(C124:G124)*$C$51</f>
         <v>4.7741116500000014E-2</v>
       </c>
-      <c r="I124" s="44"/>
+      <c r="I124" s="52"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A125" s="41">
+      <c r="A125" s="53">
         <v>16</v>
       </c>
-      <c r="B125" s="43"/>
+      <c r="B125" s="54"/>
       <c r="C125" s="19" t="s">
         <v>1</v>
       </c>
@@ -6585,13 +6910,13 @@
       <c r="H125" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I125" s="44" t="str">
+      <c r="I125" s="52" t="str">
         <f>IF(H126&gt;H127,B126,B127)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A126" s="39" t="s">
+      <c r="A126" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B126" s="14" t="s">
@@ -6621,10 +6946,10 @@
         <f>PRODUCT(C126:G126)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I126" s="44"/>
+      <c r="I126" s="52"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A127" s="42"/>
+      <c r="A127" s="51"/>
       <c r="B127" s="14" t="s">
         <v>2</v>
       </c>
@@ -6652,13 +6977,13 @@
         <f>PRODUCT(C127:G127)*$C$51</f>
         <v>3.2736765600000009E-2</v>
       </c>
-      <c r="I127" s="44"/>
+      <c r="I127" s="52"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A128" s="41">
+      <c r="A128" s="53">
         <v>17</v>
       </c>
-      <c r="B128" s="43"/>
+      <c r="B128" s="54"/>
       <c r="C128" s="19" t="s">
         <v>1</v>
       </c>
@@ -6677,13 +7002,13 @@
       <c r="H128" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I128" s="44" t="str">
+      <c r="I128" s="52" t="str">
         <f>IF(H129&gt;H130,B129,B130)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A129" s="39" t="s">
+      <c r="A129" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B129" s="14" t="s">
@@ -6713,10 +7038,10 @@
         <f>PRODUCT(C129:G129)*$C$50</f>
         <v>5.5659225600000004E-3</v>
       </c>
-      <c r="I129" s="44"/>
+      <c r="I129" s="52"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A130" s="42"/>
+      <c r="A130" s="51"/>
       <c r="B130" s="14" t="s">
         <v>2</v>
       </c>
@@ -6744,13 +7069,13 @@
         <f>PRODUCT(C130:G130)*$C$51</f>
         <v>2.7280638000000006E-2</v>
       </c>
-      <c r="I130" s="44"/>
+      <c r="I130" s="52"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A131" s="41">
+      <c r="A131" s="53">
         <v>18</v>
       </c>
-      <c r="B131" s="43"/>
+      <c r="B131" s="54"/>
       <c r="C131" s="19" t="s">
         <v>0</v>
       </c>
@@ -6769,13 +7094,13 @@
       <c r="H131" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I131" s="44" t="str">
+      <c r="I131" s="52" t="str">
         <f>IF(H132&gt;H133,B132,B133)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A132" s="39" t="s">
+      <c r="A132" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B132" s="14" t="s">
@@ -6805,10 +7130,10 @@
         <f>PRODUCT(C132:G132)*$C$50</f>
         <v>9.7403644800000012E-3</v>
       </c>
-      <c r="I132" s="44"/>
+      <c r="I132" s="52"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A133" s="42"/>
+      <c r="A133" s="51"/>
       <c r="B133" s="14" t="s">
         <v>2</v>
       </c>
@@ -6836,13 +7161,13 @@
         <f>PRODUCT(C133:G133)*$C$51</f>
         <v>2.8644669900000006E-2</v>
       </c>
-      <c r="I133" s="44"/>
+      <c r="I133" s="52"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A134" s="41">
+      <c r="A134" s="53">
         <v>19</v>
       </c>
-      <c r="B134" s="41"/>
+      <c r="B134" s="53"/>
       <c r="C134" s="19" t="s">
         <v>0</v>
       </c>
@@ -6861,13 +7186,13 @@
       <c r="H134" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I134" s="40" t="str">
+      <c r="I134" s="60" t="str">
         <f>IF(H135&gt;H136,B135,B136)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A135" s="39" t="s">
+      <c r="A135" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B135" s="14" t="s">
@@ -6897,10 +7222,10 @@
         <f>PRODUCT(C135:G135)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I135" s="40"/>
+      <c r="I135" s="60"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A136" s="39"/>
+      <c r="A136" s="50"/>
       <c r="B136" s="14" t="s">
         <v>2</v>
       </c>
@@ -6928,13 +7253,13 @@
         <f>PRODUCT(C136:G136)*$C$51</f>
         <v>2.8644669900000008E-3</v>
       </c>
-      <c r="I136" s="40"/>
+      <c r="I136" s="60"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A137" s="41">
+      <c r="A137" s="53">
         <v>20</v>
       </c>
-      <c r="B137" s="43"/>
+      <c r="B137" s="54"/>
       <c r="C137" s="19" t="s">
         <v>1</v>
       </c>
@@ -6953,13 +7278,13 @@
       <c r="H137" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I137" s="46" t="str">
+      <c r="I137" s="55" t="str">
         <f>IF(H138&gt;H139,B138,B139)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A138" s="39" t="s">
+      <c r="A138" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B138" s="14" t="s">
@@ -6989,10 +7314,10 @@
         <f>PRODUCT(C138:G138)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I138" s="47"/>
+      <c r="I138" s="56"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A139" s="42"/>
+      <c r="A139" s="51"/>
       <c r="B139" s="14" t="s">
         <v>2</v>
       </c>
@@ -7020,30 +7345,72 @@
         <f>PRODUCT(C139:G139)*$C$51</f>
         <v>1.6368382800000002E-3</v>
       </c>
-      <c r="I139" s="48"/>
+      <c r="I139" s="57"/>
     </row>
     <row r="153" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="A79:B80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="I80:I82"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:G45"/>
-    <mergeCell ref="F28:G29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="A39:B40"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="I134:I136"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="I122:I124"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="I113:I115"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="I116:I118"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="I137:I139"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="J67:K68"/>
+    <mergeCell ref="J69:K72"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="I131:I133"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="I125:I127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="I128:I130"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="I107:I109"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="I101:I103"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="I95:I97"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="I98:I100"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="I89:I91"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="I92:I94"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="I83:I85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="I86:I88"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A83:B83"/>
     <mergeCell ref="H44:K44"/>
     <mergeCell ref="H39:K39"/>
     <mergeCell ref="H34:K34"/>
@@ -7060,67 +7427,25 @@
     <mergeCell ref="F36:F37"/>
     <mergeCell ref="A28:B29"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="I83:I85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="I86:I88"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="I89:I91"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="I92:I94"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="I95:I97"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="I98:I100"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="I101:I103"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="I107:I109"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="I137:I139"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="J67:K68"/>
-    <mergeCell ref="J69:K72"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="I131:I133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="I125:I127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="I128:I130"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="I134:I136"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="I122:I124"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="I113:I115"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="I116:I118"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="F28:G29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="A39:B40"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="A79:B80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="I80:I82"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A1:A21 C2:D21">
@@ -7152,6 +7477,525 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B7A5E7-0D1D-49AD-B6BD-E47ED560C8B9}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="7" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="68">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="69">
+        <v>2</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="68">
+        <v>3</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="69">
+        <v>4</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="68">
+        <v>5</v>
+      </c>
+      <c r="B6" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="69">
+        <v>6</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="68">
+        <v>7</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="69">
+        <v>8</v>
+      </c>
+      <c r="B9" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="68">
+        <v>9</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="69">
+        <v>10</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="68">
+        <v>11</v>
+      </c>
+      <c r="B12" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="69">
+        <v>12</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="68">
+        <v>13</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="69">
+        <v>14</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="68">
+        <v>15</v>
+      </c>
+      <c r="B16" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="69">
+        <v>16</v>
+      </c>
+      <c r="B17" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="68">
+        <v>17</v>
+      </c>
+      <c r="B18" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="69">
+        <v>18</v>
+      </c>
+      <c r="B19" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="68">
+        <v>19</v>
+      </c>
+      <c r="B20" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="70">
+        <v>20</v>
+      </c>
+      <c r="B21" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="cellIs" priority="3" operator="equal">
+      <formula>"A1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C21">
+    <cfRule type="cellIs" priority="2" operator="equal">
+      <formula>"A1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D21">
+    <cfRule type="cellIs" priority="1" operator="equal">
+      <formula>"A1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A02A39-F2B8-4A72-BE6A-2B6D7673FEB4}">
   <dimension ref="A1:K57"/>
   <sheetViews>
@@ -7434,34 +8278,34 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67" t="s">
+      <c r="B11" s="62"/>
+      <c r="C11" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="67"/>
-      <c r="F11" s="66" t="s">
+      <c r="D11" s="63"/>
+      <c r="F11" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="66"/>
-      <c r="H11" s="67" t="s">
+      <c r="G11" s="62"/>
+      <c r="H11" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="67"/>
+      <c r="I11" s="63"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="66"/>
-      <c r="B12" s="66"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
       <c r="H12" s="16" t="s">
         <v>3</v>
       </c>
@@ -7470,7 +8314,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="61" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -7482,7 +8326,7 @@
       <c r="D13" s="20">
         <v>0.77</v>
       </c>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="61" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="17" t="s">
@@ -7496,7 +8340,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="65"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="17" t="s">
         <v>1</v>
       </c>
@@ -7506,7 +8350,7 @@
       <c r="D14" s="20">
         <v>0.44</v>
       </c>
-      <c r="F14" s="65"/>
+      <c r="F14" s="61"/>
       <c r="G14" s="17" t="s">
         <v>13</v>
       </c>
@@ -7522,7 +8366,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="F15" s="65"/>
+      <c r="F15" s="61"/>
       <c r="G15" s="17" t="s">
         <v>14</v>
       </c>
@@ -7534,34 +8378,34 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="67" t="s">
+      <c r="B17" s="62"/>
+      <c r="C17" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="67"/>
-      <c r="F17" s="66" t="s">
+      <c r="D17" s="63"/>
+      <c r="F17" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="66"/>
-      <c r="H17" s="67" t="s">
+      <c r="G17" s="62"/>
+      <c r="H17" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="67"/>
+      <c r="I17" s="63"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="66"/>
-      <c r="B18" s="66"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="62"/>
       <c r="C18" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
       <c r="H18" s="16" t="s">
         <v>3</v>
       </c>
@@ -7570,7 +8414,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="61" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -7582,7 +8426,7 @@
       <c r="D19" s="20">
         <v>0.09</v>
       </c>
-      <c r="F19" s="65" t="s">
+      <c r="F19" s="61" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="17" t="s">
@@ -7596,7 +8440,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="65"/>
+      <c r="A20" s="61"/>
       <c r="B20" s="17" t="s">
         <v>2</v>
       </c>
@@ -7606,7 +8450,7 @@
       <c r="D20" s="20">
         <v>0.9</v>
       </c>
-      <c r="F20" s="65"/>
+      <c r="F20" s="61"/>
       <c r="G20" s="17" t="s">
         <v>30</v>
       </c>
@@ -7624,14 +8468,14 @@
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="67" t="s">
+      <c r="B22" s="62"/>
+      <c r="C22" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="67"/>
+      <c r="D22" s="63"/>
       <c r="F22" s="20"/>
       <c r="G22" s="64" t="s">
         <v>34</v>
@@ -7639,8 +8483,8 @@
       <c r="H22" s="64"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="66"/>
-      <c r="B23" s="66"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="62"/>
       <c r="C23" s="16" t="s">
         <v>3</v>
       </c>
@@ -7660,7 +8504,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="61" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -7685,7 +8529,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="65"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="17" t="s">
         <v>2</v>
       </c>
@@ -7762,10 +8606,10 @@
       <c r="H28" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J28" s="49" t="s">
+      <c r="J28" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="K28" s="49"/>
+      <c r="K28" s="58"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="29">
@@ -7792,8 +8636,8 @@
       <c r="H29" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="27">
@@ -7820,11 +8664,11 @@
       <c r="H30" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J30" s="61">
+      <c r="J30" s="67">
         <f>6/7*100</f>
         <v>85.714285714285708</v>
       </c>
-      <c r="K30" s="61"/>
+      <c r="K30" s="67"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="29">
@@ -7851,8 +8695,8 @@
       <c r="H31" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="61"/>
-      <c r="K31" s="61"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="27">
@@ -7879,8 +8723,8 @@
       <c r="H32" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="29">
@@ -7907,8 +8751,8 @@
       <c r="H33" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="27">
@@ -7937,10 +8781,10 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="54">
+      <c r="A36" s="36">
         <v>1</v>
       </c>
-      <c r="B36" s="54"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="22" t="s">
         <v>17</v>
       </c>
@@ -7964,8 +8808,8 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="54"/>
-      <c r="B37" s="54"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="23" t="s">
         <v>1</v>
       </c>
@@ -7984,13 +8828,13 @@
       <c r="H37" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="44" t="str">
+      <c r="I37" s="52" t="str">
         <f>IF(H38&gt;H39,B38,B39)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="55" t="s">
+      <c r="A38" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B38" s="14" t="s">
@@ -8020,10 +8864,10 @@
         <f>PRODUCT(C38:G38)*$H$23</f>
         <v>2.3191344000000003E-2</v>
       </c>
-      <c r="I38" s="44"/>
+      <c r="I38" s="52"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="55"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="14" t="s">
         <v>2</v>
       </c>
@@ -8051,13 +8895,13 @@
         <f>PRODUCT(C39:G39)*$H$24</f>
         <v>3.4642079999999995E-4</v>
       </c>
-      <c r="I39" s="44"/>
+      <c r="I39" s="52"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="62">
-        <v>2</v>
-      </c>
-      <c r="B40" s="63"/>
+      <c r="A40" s="65">
+        <v>2</v>
+      </c>
+      <c r="B40" s="66"/>
       <c r="C40" s="23" t="s">
         <v>0</v>
       </c>
@@ -8076,13 +8920,13 @@
       <c r="H40" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I40" s="44" t="str">
+      <c r="I40" s="52" t="str">
         <f>IF(H41&gt;H42,B41,B42)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="55" t="s">
+      <c r="A41" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="14" t="s">
@@ -8112,10 +8956,10 @@
         <f>PRODUCT(C41:G41)*$H$23</f>
         <v>1.4494590000000002E-2</v>
       </c>
-      <c r="I41" s="44"/>
+      <c r="I41" s="52"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="55"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="14" t="s">
         <v>2</v>
       </c>
@@ -8143,13 +8987,13 @@
         <f>PRODUCT(C42:G42)*$H$24</f>
         <v>6.9284159999999991E-4</v>
       </c>
-      <c r="I42" s="44"/>
+      <c r="I42" s="52"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="62">
-        <v>3</v>
-      </c>
-      <c r="B43" s="63"/>
+      <c r="A43" s="65">
+        <v>3</v>
+      </c>
+      <c r="B43" s="66"/>
       <c r="C43" s="23" t="s">
         <v>1</v>
       </c>
@@ -8168,13 +9012,13 @@
       <c r="H43" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I43" s="44" t="str">
+      <c r="I43" s="52" t="str">
         <f>IF(H44&gt;H45,B44,B45)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -8204,10 +9048,10 @@
         <f>PRODUCT(C44:G44)*$H$23</f>
         <v>4.6382688000000004E-3</v>
       </c>
-      <c r="I44" s="44"/>
+      <c r="I44" s="52"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="55"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="14" t="s">
         <v>2</v>
       </c>
@@ -8235,13 +9079,13 @@
         <f>PRODUCT(C45:G45)*$H$24</f>
         <v>2.3094719999999999E-3</v>
       </c>
-      <c r="I45" s="44"/>
+      <c r="I45" s="52"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="62">
+      <c r="A46" s="65">
         <v>4</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="66"/>
       <c r="C46" s="23" t="s">
         <v>1</v>
       </c>
@@ -8260,13 +9104,13 @@
       <c r="H46" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I46" s="45" t="str">
+      <c r="I46" s="43" t="str">
         <f>IF(H47&gt;H48,B47,B48)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="55" t="s">
+      <c r="A47" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B47" s="14" t="s">
@@ -8296,10 +9140,10 @@
         <f>PRODUCT(C47:G47)*$H$23</f>
         <v>2.3191344000000003E-2</v>
       </c>
-      <c r="I47" s="45"/>
+      <c r="I47" s="43"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="55"/>
+      <c r="A48" s="37"/>
       <c r="B48" s="14" t="s">
         <v>2</v>
       </c>
@@ -8327,13 +9171,13 @@
         <f>PRODUCT(C48:G48)*$H$24</f>
         <v>3.4642079999999995E-4</v>
       </c>
-      <c r="I48" s="45"/>
+      <c r="I48" s="43"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="62">
+      <c r="A49" s="65">
         <v>5</v>
       </c>
-      <c r="B49" s="63"/>
+      <c r="B49" s="66"/>
       <c r="C49" s="23" t="s">
         <v>0</v>
       </c>
@@ -8352,13 +9196,13 @@
       <c r="H49" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I49" s="44" t="str">
+      <c r="I49" s="52" t="str">
         <f>IF(H50&gt;H51,B50,B51)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="55" t="s">
+      <c r="A50" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -8388,10 +9232,10 @@
         <f>PRODUCT(C50:G50)*$H$23</f>
         <v>2.3191344000000002E-3</v>
       </c>
-      <c r="I50" s="44"/>
+      <c r="I50" s="52"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="55"/>
+      <c r="A51" s="37"/>
       <c r="B51" s="14" t="s">
         <v>2</v>
       </c>
@@ -8419,13 +9263,13 @@
         <f>PRODUCT(C51:G51)*$H$24</f>
         <v>4.0415759999999998E-3</v>
       </c>
-      <c r="I51" s="44"/>
+      <c r="I51" s="52"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="62">
+      <c r="A52" s="65">
         <v>6</v>
       </c>
-      <c r="B52" s="63"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="23" t="s">
         <v>1</v>
       </c>
@@ -8444,13 +9288,13 @@
       <c r="H52" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I52" s="44" t="str">
+      <c r="I52" s="52" t="str">
         <f>IF(H53&gt;H54,B53,B54)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="55" t="s">
+      <c r="A53" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B53" s="14" t="s">
@@ -8480,10 +9324,10 @@
         <f>PRODUCT(C53:G53)*$H$23</f>
         <v>1.6565245714285713E-3</v>
       </c>
-      <c r="I53" s="44"/>
+      <c r="I53" s="52"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="55"/>
+      <c r="A54" s="37"/>
       <c r="B54" s="14" t="s">
         <v>2</v>
       </c>
@@ -8511,13 +9355,13 @@
         <f>PRODUCT(C54:G54)*$H$24</f>
         <v>1.3196982857142856E-2</v>
       </c>
-      <c r="I54" s="44"/>
+      <c r="I54" s="52"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="62">
+      <c r="A55" s="65">
         <v>7</v>
       </c>
-      <c r="B55" s="63"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="23" t="s">
         <v>0</v>
       </c>
@@ -8536,13 +9380,13 @@
       <c r="H55" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I55" s="44" t="str">
+      <c r="I55" s="52" t="str">
         <f>IF(H56&gt;H57,B56,B57)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="55" t="s">
+      <c r="A56" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B56" s="14" t="s">
@@ -8572,10 +9416,10 @@
         <f>PRODUCT(C56:G56)*$H$23</f>
         <v>2.6504393142857143E-3</v>
       </c>
-      <c r="I56" s="44"/>
+      <c r="I56" s="52"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="55"/>
+      <c r="A57" s="37"/>
       <c r="B57" s="14" t="s">
         <v>2</v>
       </c>
@@ -8603,10 +9447,34 @@
         <f>PRODUCT(C57:G57)*$H$24</f>
         <v>0.12124728000000001</v>
       </c>
-      <c r="I57" s="44"/>
+      <c r="I57" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="J28:K29"/>
+    <mergeCell ref="J30:K33"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="I43:I45"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="I55:I57"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="A50:A51"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A17:B18"/>
     <mergeCell ref="C17:D17"/>
@@ -8623,30 +9491,6 @@
     <mergeCell ref="F17:G18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="I55:I57"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="J28:K29"/>
-    <mergeCell ref="J30:K33"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="I43:I45"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CLEAN: refactor code and file
</commit_message>
<xml_diff>
--- a/uploads/dataset.xlsx
+++ b/uploads/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iqbal al-ayyubi\Documents\upn-jatim\semester 3\Statkom\naive-bayes-app\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816D083E-D369-4EAC-A14D-F45EACA6BB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8CB5B3-CA8E-4D4A-ADD4-3771BAA18779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATASET" sheetId="1" r:id="rId1"/>
@@ -926,7 +926,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1023,10 +1023,70 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="10" xfId="32" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="23" xfId="25" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="16" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="24" xfId="25" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="22" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="24" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="28" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="23" applyBorder="1" applyAlignment="1">
@@ -1050,71 +1110,8 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="15" xfId="24" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="28" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="23" xfId="25" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="24" xfId="25" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="16" xfId="23" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="23" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="22" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="24" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="23" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="10" xfId="22" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="29" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="10" xfId="30" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="24" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="25" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1122,16 +1119,16 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="28" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="2" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="29" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="10" xfId="22" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="10" xfId="30" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="24" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1180,294 +1177,6 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="65">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1883,6 +1592,294 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2055,50 +2052,50 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3B840F97-9D3E-4002-8C65-50C00E9E68B6}" name="Table4" displayName="Table4" ref="A1:G21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3B840F97-9D3E-4002-8C65-50C00E9E68B6}" name="Table4" displayName="Table4" ref="A1:G21" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="A1:G21" xr:uid="{3B840F97-9D3E-4002-8C65-50C00E9E68B6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EBDB54CD-4136-44A2-A5D8-16D6A7FDFEF6}" name="No" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{A51E0D62-F7AE-4CF5-AB71-B0970ED0A5C1}" name="A1" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{28AEF9E7-B4DC-4C35-B9B1-42FB8D0CD93F}" name="A3" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{821674A5-3142-4BB7-A3D6-3009C13EBE3F}" name="A4" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{4C341E52-534C-4DA0-9857-2E54F276D560}" name="A5" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{7994CE9D-28B4-410B-95AA-5D1276DC5454}" name="A7" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{862BF86E-35D0-41F0-8FA0-FE9EC6C5BA15}" name="Kelas" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EBDB54CD-4136-44A2-A5D8-16D6A7FDFEF6}" name="No" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{A51E0D62-F7AE-4CF5-AB71-B0970ED0A5C1}" name="A1" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{28AEF9E7-B4DC-4C35-B9B1-42FB8D0CD93F}" name="A3" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{821674A5-3142-4BB7-A3D6-3009C13EBE3F}" name="A4" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{4C341E52-534C-4DA0-9857-2E54F276D560}" name="A5" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{7994CE9D-28B4-410B-95AA-5D1276DC5454}" name="A7" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{862BF86E-35D0-41F0-8FA0-FE9EC6C5BA15}" name="Kelas" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E43C5A67-0B0E-4FC9-88BC-F5BCF9409F37}" name="Table3" displayName="Table3" ref="A1:H8" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E43C5A67-0B0E-4FC9-88BC-F5BCF9409F37}" name="Table3" displayName="Table3" ref="A1:H8" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <autoFilter ref="A1:H8" xr:uid="{E43C5A67-0B0E-4FC9-88BC-F5BCF9409F37}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D57249E6-A2DD-443B-96EF-7E2A50FE96EE}" name="A1" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{210CD1B4-4A40-48CB-BE25-18CAB49D43C2}" name="A2" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{3312FDAA-8C88-44BB-88D5-B188BDC0F26D}" name="A3" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{5995CFA6-6AD2-4936-998F-2AA16B2B3EA1}" name="A4" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{092C32B2-067B-476E-A4D3-2F7762D153C1}" name="A5" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{042C6AC1-6CCA-4920-85E5-614E885036FF}" name="A6" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{ECE2C959-8E6A-4733-A47E-8F83388B4903}" name="A7" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{C9EA31FF-440C-4B76-823B-CCAB36E71730}" name="Kelas" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{D57249E6-A2DD-443B-96EF-7E2A50FE96EE}" name="A1" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{210CD1B4-4A40-48CB-BE25-18CAB49D43C2}" name="A2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{3312FDAA-8C88-44BB-88D5-B188BDC0F26D}" name="A3" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{5995CFA6-6AD2-4936-998F-2AA16B2B3EA1}" name="A4" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{092C32B2-067B-476E-A4D3-2F7762D153C1}" name="A5" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{042C6AC1-6CCA-4920-85E5-614E885036FF}" name="A6" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{ECE2C959-8E6A-4733-A47E-8F83388B4903}" name="A7" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{C9EA31FF-440C-4B76-823B-CCAB36E71730}" name="Kelas" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A14F7FD6-DC4E-4509-A422-2947C1FD40F1}" name="Table8" displayName="Table8" ref="A27:H34" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A14F7FD6-DC4E-4509-A422-2947C1FD40F1}" name="Table8" displayName="Table8" ref="A27:H34" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A27:H34" xr:uid="{A14F7FD6-DC4E-4509-A422-2947C1FD40F1}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{44CE8644-5295-432D-8B3F-EE68F19519DB}" name="No" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{32A7D7FA-4120-46AA-9921-71C36BFB5E4F}" name="A1" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{E43E2477-B25B-4F31-8D78-B5E79037476A}" name="A3" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{321D3E0C-2282-4D82-A4BA-A11F380E5562}" name="A4" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{019591A9-F012-4A73-BA2D-DEBC506C80F8}" name="A5" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{6403F498-3368-417E-9BB5-030E5CA84CF0}" name="A7" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{CC3D58F9-0B78-424C-8483-09CBB1789DB2}" name="Kelas" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{6BFBC307-003C-422A-AAFC-F1B43CD635DC}" name="Prediction" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{44CE8644-5295-432D-8B3F-EE68F19519DB}" name="No" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{32A7D7FA-4120-46AA-9921-71C36BFB5E4F}" name="A1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E43E2477-B25B-4F31-8D78-B5E79037476A}" name="A3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{321D3E0C-2282-4D82-A4BA-A11F380E5562}" name="A4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{019591A9-F012-4A73-BA2D-DEBC506C80F8}" name="A5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{6403F498-3368-417E-9BB5-030E5CA84CF0}" name="A7" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{CC3D58F9-0B78-424C-8483-09CBB1789DB2}" name="Kelas" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{6BFBC307-003C-422A-AAFC-F1B43CD635DC}" name="Prediction" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2447,10 +2444,10 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="35"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3203,10 +3200,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="34"/>
+      <c r="B30" s="36"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
@@ -3216,10 +3213,10 @@
         <f>COUNT(Table1[A2])</f>
         <v>27</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="36"/>
       <c r="F31" s="5" t="s">
         <v>9</v>
       </c>
@@ -3312,14 +3309,14 @@
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="34"/>
-      <c r="D38" s="34" t="s">
+      <c r="B38" s="36"/>
+      <c r="D38" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="34"/>
+      <c r="E38" s="36"/>
       <c r="F38" s="5" t="s">
         <v>9</v>
       </c>
@@ -3535,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D884DC29-9C63-4ED2-98E5-F89FE5DACB23}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I95" sqref="I95:I97"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3580,10 +3577,10 @@
       <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="35"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -4154,29 +4151,29 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45" t="s">
+      <c r="B23" s="53"/>
+      <c r="C23" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="45"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="46"/>
-      <c r="H23" s="47" t="s">
+      <c r="G23" s="55"/>
+      <c r="H23" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="49"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="40"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="13" t="s">
         <v>3</v>
       </c>
@@ -4184,8 +4181,8 @@
         <v>2</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
       <c r="H24" s="13" t="s">
         <v>3</v>
       </c>
@@ -4196,7 +4193,7 @@
       <c r="K24" s="13"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="37" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -4211,7 +4208,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="37" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -4235,7 +4232,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="35"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="3" t="s">
         <v>1</v>
       </c>
@@ -4248,7 +4245,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="35"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="3" t="s">
         <v>1</v>
       </c>
@@ -4279,29 +4276,29 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="45" t="s">
+      <c r="B28" s="53"/>
+      <c r="C28" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="45"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="46"/>
-      <c r="H28" s="47" t="s">
+      <c r="G28" s="55"/>
+      <c r="H28" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="49"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="13" t="s">
         <v>3</v>
       </c>
@@ -4309,8 +4306,8 @@
         <v>2</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
       <c r="H29" s="13" t="s">
         <v>3</v>
       </c>
@@ -4321,7 +4318,7 @@
       <c r="K29" s="13"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="37" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -4336,7 +4333,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="37" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -4360,7 +4357,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="35"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="3" t="s">
         <v>13</v>
       </c>
@@ -4373,7 +4370,7 @@
         <v>3</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="35"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="3" t="s">
         <v>13</v>
       </c>
@@ -4395,7 +4392,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="35"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
@@ -4408,7 +4405,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="35"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="3" t="s">
         <v>14</v>
       </c>
@@ -4439,29 +4436,29 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="45" t="s">
+      <c r="B34" s="53"/>
+      <c r="C34" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="45"/>
+      <c r="D34" s="54"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="46"/>
-      <c r="H34" s="47" t="s">
+      <c r="G34" s="55"/>
+      <c r="H34" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="49"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="40"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A35" s="44"/>
-      <c r="B35" s="44"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="53"/>
       <c r="C35" s="13" t="s">
         <v>3</v>
       </c>
@@ -4469,8 +4466,8 @@
         <v>2</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
       <c r="H35" s="13" t="s">
         <v>3</v>
       </c>
@@ -4481,7 +4478,7 @@
       <c r="K35" s="13"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="37" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -4496,7 +4493,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="35" t="s">
+      <c r="F36" s="37" t="s">
         <v>24</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -4520,7 +4517,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="35"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="3" t="s">
         <v>2</v>
       </c>
@@ -4533,7 +4530,7 @@
         <v>10</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="35"/>
+      <c r="F37" s="37"/>
       <c r="G37" s="3" t="s">
         <v>2</v>
       </c>
@@ -4564,29 +4561,29 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="45" t="s">
+      <c r="B39" s="53"/>
+      <c r="C39" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="45"/>
+      <c r="D39" s="54"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="46" t="s">
+      <c r="F39" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="46"/>
-      <c r="H39" s="47" t="s">
+      <c r="G39" s="55"/>
+      <c r="H39" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="49"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="40"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="44"/>
-      <c r="B40" s="44"/>
+      <c r="A40" s="53"/>
+      <c r="B40" s="53"/>
       <c r="C40" s="13" t="s">
         <v>3</v>
       </c>
@@ -4594,8 +4591,8 @@
         <v>2</v>
       </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
       <c r="H40" s="13" t="s">
         <v>3</v>
       </c>
@@ -4606,7 +4603,7 @@
       <c r="K40" s="13"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="37" t="s">
         <v>25</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -4621,7 +4618,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="37" t="s">
         <v>25</v>
       </c>
       <c r="G41" s="3" t="s">
@@ -4645,7 +4642,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="35"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="3" t="s">
         <v>2</v>
       </c>
@@ -4658,7 +4655,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="35"/>
+      <c r="F42" s="37"/>
       <c r="G42" s="3" t="s">
         <v>2</v>
       </c>
@@ -4689,29 +4686,29 @@
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="44"/>
-      <c r="C44" s="45" t="s">
+      <c r="B44" s="53"/>
+      <c r="C44" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="45"/>
+      <c r="D44" s="54"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="46" t="s">
+      <c r="F44" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="G44" s="46"/>
-      <c r="H44" s="47" t="s">
+      <c r="G44" s="55"/>
+      <c r="H44" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="49"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="40"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="44"/>
-      <c r="B45" s="44"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="13" t="s">
         <v>3</v>
       </c>
@@ -4719,8 +4716,8 @@
         <v>2</v>
       </c>
       <c r="E45" s="1"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
       <c r="H45" s="13" t="s">
         <v>3</v>
       </c>
@@ -4731,7 +4728,7 @@
       <c r="K45" s="13"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="37" t="s">
         <v>26</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -4746,7 +4743,7 @@
         <v>7</v>
       </c>
       <c r="E46" s="1"/>
-      <c r="F46" s="35" t="s">
+      <c r="F46" s="37" t="s">
         <v>26</v>
       </c>
       <c r="G46" s="3" t="s">
@@ -4770,7 +4767,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="35"/>
+      <c r="A47" s="37"/>
       <c r="B47" s="3" t="s">
         <v>30</v>
       </c>
@@ -4783,7 +4780,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="1"/>
-      <c r="F47" s="35"/>
+      <c r="F47" s="37"/>
       <c r="G47" s="3" t="s">
         <v>30</v>
       </c>
@@ -4806,11 +4803,11 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
@@ -4856,20 +4853,20 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
-      <c r="J55" s="35" t="s">
+      <c r="B55" s="59"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="60"/>
+      <c r="J55" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="K55" s="35"/>
+      <c r="K55" s="37"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
@@ -5230,10 +5227,10 @@
       <c r="H67" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J67" s="58" t="s">
+      <c r="J67" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="K67" s="58"/>
+      <c r="K67" s="50"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="7">
@@ -5260,8 +5257,8 @@
       <c r="H68" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J68" s="58"/>
-      <c r="K68" s="58"/>
+      <c r="J68" s="50"/>
+      <c r="K68" s="50"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="7">
@@ -5288,11 +5285,11 @@
       <c r="H69" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J69" s="59">
+      <c r="J69" s="51">
         <f>17/20*100</f>
         <v>85</v>
       </c>
-      <c r="K69" s="59"/>
+      <c r="K69" s="51"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="7">
@@ -5319,8 +5316,8 @@
       <c r="H70" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J70" s="59"/>
-      <c r="K70" s="59"/>
+      <c r="J70" s="51"/>
+      <c r="K70" s="51"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="7">
@@ -5347,8 +5344,8 @@
       <c r="H71" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J71" s="59"/>
-      <c r="K71" s="59"/>
+      <c r="J71" s="51"/>
+      <c r="K71" s="51"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="7">
@@ -5375,8 +5372,8 @@
       <c r="H72" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J72" s="59"/>
-      <c r="K72" s="59"/>
+      <c r="J72" s="51"/>
+      <c r="K72" s="51"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="7">
@@ -5483,10 +5480,10 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79" s="36">
+      <c r="A79" s="56">
         <v>1</v>
       </c>
-      <c r="B79" s="36"/>
+      <c r="B79" s="56"/>
       <c r="C79" s="22" t="s">
         <v>17</v>
       </c>
@@ -5510,8 +5507,8 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A80" s="36"/>
-      <c r="B80" s="36"/>
+      <c r="A80" s="56"/>
+      <c r="B80" s="56"/>
       <c r="C80" s="23" t="s">
         <v>0</v>
       </c>
@@ -5530,13 +5527,13 @@
       <c r="H80" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="43" t="str">
+      <c r="I80" s="52" t="str">
         <f>IF(H81&gt;H82,B81,B82)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="37" t="s">
+      <c r="A81" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B81" s="14" t="s">
@@ -5566,10 +5563,10 @@
         <f>PRODUCT(C81:G81)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I81" s="43"/>
+      <c r="I81" s="52"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="37"/>
+      <c r="A82" s="57"/>
       <c r="B82" s="14" t="s">
         <v>2</v>
       </c>
@@ -5597,13 +5594,13 @@
         <f>PRODUCT(C82:G82)*$C$51</f>
         <v>3.2736765600000009E-2</v>
       </c>
-      <c r="I82" s="43"/>
+      <c r="I82" s="52"/>
     </row>
     <row r="83" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="53">
-        <v>2</v>
-      </c>
-      <c r="B83" s="54"/>
+      <c r="A83" s="43">
+        <v>2</v>
+      </c>
+      <c r="B83" s="45"/>
       <c r="C83" s="19" t="s">
         <v>1</v>
       </c>
@@ -5622,13 +5619,13 @@
       <c r="H83" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I83" s="52" t="str">
+      <c r="I83" s="46" t="str">
         <f>IF(H84&gt;H85,B84,B85)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84" s="50" t="s">
+      <c r="A84" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B84" s="14" t="s">
@@ -5658,10 +5655,10 @@
         <f>PRODUCT(C84:G84)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I84" s="52"/>
+      <c r="I84" s="46"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" s="51"/>
+      <c r="A85" s="44"/>
       <c r="B85" s="14" t="s">
         <v>2</v>
       </c>
@@ -5689,13 +5686,13 @@
         <f>PRODUCT(C85:G85)*$C$51</f>
         <v>1.8706723200000004E-2</v>
       </c>
-      <c r="I85" s="52"/>
+      <c r="I85" s="46"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86" s="53">
-        <v>3</v>
-      </c>
-      <c r="B86" s="54"/>
+      <c r="A86" s="43">
+        <v>3</v>
+      </c>
+      <c r="B86" s="45"/>
       <c r="C86" s="19" t="s">
         <v>1</v>
       </c>
@@ -5714,13 +5711,13 @@
       <c r="H86" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I86" s="52" t="str">
+      <c r="I86" s="46" t="str">
         <f>IF(H87&gt;H88,B87,B88)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87" s="50" t="s">
+      <c r="A87" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B87" s="14" t="s">
@@ -5750,10 +5747,10 @@
         <f>PRODUCT(C87:G87)*$C$50</f>
         <v>3.0438639000000003E-2</v>
       </c>
-      <c r="I87" s="52"/>
+      <c r="I87" s="46"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="51"/>
+      <c r="A88" s="44"/>
       <c r="B88" s="14" t="s">
         <v>2</v>
       </c>
@@ -5781,13 +5778,13 @@
         <f>PRODUCT(C88:G88)*$C$51</f>
         <v>9.3533616000000016E-4</v>
       </c>
-      <c r="I88" s="52"/>
+      <c r="I88" s="46"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A89" s="53">
+      <c r="A89" s="43">
         <v>4</v>
       </c>
-      <c r="B89" s="54"/>
+      <c r="B89" s="45"/>
       <c r="C89" s="19" t="s">
         <v>0</v>
       </c>
@@ -5806,13 +5803,13 @@
       <c r="H89" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I89" s="43" t="str">
+      <c r="I89" s="52" t="str">
         <f>IF(H90&gt;H91,B90,B91)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A90" s="50" t="s">
+      <c r="A90" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B90" s="14" t="s">
@@ -5842,10 +5839,10 @@
         <f>PRODUCT(C90:G90)*$C$50</f>
         <v>2.4350911200000003E-3</v>
       </c>
-      <c r="I90" s="43"/>
+      <c r="I90" s="52"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91" s="51"/>
+      <c r="A91" s="44"/>
       <c r="B91" s="14" t="s">
         <v>2</v>
       </c>
@@ -5873,13 +5870,13 @@
         <f>PRODUCT(C91:G91)*$C$51</f>
         <v>1.9096446600000004E-2</v>
       </c>
-      <c r="I91" s="43"/>
+      <c r="I91" s="52"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92" s="53">
+      <c r="A92" s="43">
         <v>5</v>
       </c>
-      <c r="B92" s="54"/>
+      <c r="B92" s="45"/>
       <c r="C92" s="19" t="s">
         <v>0</v>
       </c>
@@ -5898,13 +5895,13 @@
       <c r="H92" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I92" s="52" t="str">
+      <c r="I92" s="46" t="str">
         <f>IF(H93&gt;H94,B93,B94)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" s="50" t="s">
+      <c r="A93" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B93" s="14" t="s">
@@ -5934,10 +5931,10 @@
         <f>PRODUCT(C93:G93)*$C$50</f>
         <v>3.8048298750000004E-3</v>
       </c>
-      <c r="I93" s="52"/>
+      <c r="I93" s="46"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94" s="51"/>
+      <c r="A94" s="44"/>
       <c r="B94" s="14" t="s">
         <v>2</v>
       </c>
@@ -5965,13 +5962,13 @@
         <f>PRODUCT(C94:G94)*$C$51</f>
         <v>9.0935460000000001E-4</v>
       </c>
-      <c r="I94" s="52"/>
+      <c r="I94" s="46"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A95" s="53">
+      <c r="A95" s="43">
         <v>6</v>
       </c>
-      <c r="B95" s="54"/>
+      <c r="B95" s="45"/>
       <c r="C95" s="19" t="s">
         <v>1</v>
       </c>
@@ -5990,13 +5987,13 @@
       <c r="H95" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I95" s="52" t="str">
+      <c r="I95" s="46" t="str">
         <f>IF(H96&gt;H97,B96,B97)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" s="50" t="s">
+      <c r="A96" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B96" s="14" t="s">
@@ -6026,10 +6023,10 @@
         <f>PRODUCT(C96:G96)*$C$50</f>
         <v>6.0877278000000005E-3</v>
       </c>
-      <c r="I96" s="52"/>
+      <c r="I96" s="46"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A97" s="51"/>
+      <c r="A97" s="44"/>
       <c r="B97" s="14" t="s">
         <v>2</v>
       </c>
@@ -6057,13 +6054,13 @@
         <f>PRODUCT(C97:G97)*$C$51</f>
         <v>5.1963119999999998E-3</v>
       </c>
-      <c r="I97" s="52"/>
+      <c r="I97" s="46"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A98" s="53">
+      <c r="A98" s="43">
         <v>7</v>
       </c>
-      <c r="B98" s="54"/>
+      <c r="B98" s="45"/>
       <c r="C98" s="19" t="s">
         <v>1</v>
       </c>
@@ -6082,13 +6079,13 @@
       <c r="H98" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I98" s="43" t="str">
+      <c r="I98" s="52" t="str">
         <f>IF(H99&gt;H100,B99,B100)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" s="50" t="s">
+      <c r="A99" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B99" s="14" t="s">
@@ -6118,10 +6115,10 @@
         <f>PRODUCT(C99:G99)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I99" s="43"/>
+      <c r="I99" s="52"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" s="51"/>
+      <c r="A100" s="44"/>
       <c r="B100" s="14" t="s">
         <v>2</v>
       </c>
@@ -6149,13 +6146,13 @@
         <f>PRODUCT(C100:G100)*$C$51</f>
         <v>3.2736765600000009E-2</v>
       </c>
-      <c r="I100" s="43"/>
+      <c r="I100" s="52"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A101" s="53">
+      <c r="A101" s="43">
         <v>8</v>
       </c>
-      <c r="B101" s="54"/>
+      <c r="B101" s="45"/>
       <c r="C101" s="19" t="s">
         <v>1</v>
       </c>
@@ -6174,13 +6171,13 @@
       <c r="H101" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I101" s="52" t="str">
+      <c r="I101" s="46" t="str">
         <f>IF(H102&gt;H103,B102,B103)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A102" s="50" t="s">
+      <c r="A102" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B102" s="14" t="s">
@@ -6210,10 +6207,10 @@
         <f>PRODUCT(C102:G102)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I102" s="52"/>
+      <c r="I102" s="46"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A103" s="51"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="14" t="s">
         <v>2</v>
       </c>
@@ -6241,13 +6238,13 @@
         <f>PRODUCT(C103:G103)*$C$51</f>
         <v>3.2736765600000005E-3</v>
       </c>
-      <c r="I103" s="52"/>
+      <c r="I103" s="46"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A104" s="53">
+      <c r="A104" s="43">
         <v>9</v>
       </c>
-      <c r="B104" s="54"/>
+      <c r="B104" s="45"/>
       <c r="C104" s="19" t="s">
         <v>0</v>
       </c>
@@ -6266,13 +6263,13 @@
       <c r="H104" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I104" s="52" t="str">
+      <c r="I104" s="46" t="str">
         <f>IF(H105&gt;H106,B105,B106)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A105" s="50" t="s">
+      <c r="A105" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B105" s="14" t="s">
@@ -6302,10 +6299,10 @@
         <f>PRODUCT(C105:G105)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I105" s="52"/>
+      <c r="I105" s="46"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A106" s="51"/>
+      <c r="A106" s="44"/>
       <c r="B106" s="14" t="s">
         <v>2</v>
       </c>
@@ -6333,13 +6330,13 @@
         <f>PRODUCT(C106:G106)*$C$51</f>
         <v>2.8644669900000008E-3</v>
       </c>
-      <c r="I106" s="52"/>
+      <c r="I106" s="46"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A107" s="53">
+      <c r="A107" s="43">
         <v>10</v>
       </c>
-      <c r="B107" s="54"/>
+      <c r="B107" s="45"/>
       <c r="C107" s="19" t="s">
         <v>1</v>
       </c>
@@ -6358,13 +6355,13 @@
       <c r="H107" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I107" s="52" t="str">
+      <c r="I107" s="46" t="str">
         <f>IF(H108&gt;H109,B108,B109)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A108" s="50" t="s">
+      <c r="A108" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B108" s="14" t="s">
@@ -6394,10 +6391,10 @@
         <f>PRODUCT(C108:G108)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I108" s="52"/>
+      <c r="I108" s="46"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A109" s="51"/>
+      <c r="A109" s="44"/>
       <c r="B109" s="14" t="s">
         <v>2</v>
       </c>
@@ -6425,13 +6422,13 @@
         <f>PRODUCT(C109:G109)*$C$51</f>
         <v>1.6368382800000005E-2</v>
       </c>
-      <c r="I109" s="52"/>
+      <c r="I109" s="46"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A110" s="53">
+      <c r="A110" s="43">
         <v>11</v>
       </c>
-      <c r="B110" s="54"/>
+      <c r="B110" s="45"/>
       <c r="C110" s="19" t="s">
         <v>0</v>
       </c>
@@ -6450,13 +6447,13 @@
       <c r="H110" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I110" s="52" t="str">
+      <c r="I110" s="46" t="str">
         <f>IF(H111&gt;H112,B111,B112)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A111" s="50" t="s">
+      <c r="A111" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B111" s="14" t="s">
@@ -6486,10 +6483,10 @@
         <f>PRODUCT(C111:G111)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I111" s="52"/>
+      <c r="I111" s="46"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A112" s="51"/>
+      <c r="A112" s="44"/>
       <c r="B112" s="14" t="s">
         <v>2</v>
       </c>
@@ -6517,13 +6514,13 @@
         <f>PRODUCT(C112:G112)*$C$51</f>
         <v>2.7280638000000006E-2</v>
       </c>
-      <c r="I112" s="52"/>
+      <c r="I112" s="46"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113" s="53">
+      <c r="A113" s="43">
         <v>12</v>
       </c>
-      <c r="B113" s="54"/>
+      <c r="B113" s="45"/>
       <c r="C113" s="19" t="s">
         <v>1</v>
       </c>
@@ -6542,13 +6539,13 @@
       <c r="H113" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I113" s="52" t="str">
+      <c r="I113" s="46" t="str">
         <f>IF(H114&gt;H115,B114,B115)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114" s="50" t="s">
+      <c r="A114" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B114" s="14" t="s">
@@ -6578,10 +6575,10 @@
         <f>PRODUCT(C114:G114)*$C$50</f>
         <v>6.9574032000000001E-3</v>
       </c>
-      <c r="I114" s="52"/>
+      <c r="I114" s="46"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="51"/>
+      <c r="A115" s="44"/>
       <c r="B115" s="14" t="s">
         <v>2</v>
       </c>
@@ -6609,13 +6606,13 @@
         <f>PRODUCT(C115:G115)*$C$51</f>
         <v>1.5588936000000003E-2</v>
       </c>
-      <c r="I115" s="52"/>
+      <c r="I115" s="46"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="53">
+      <c r="A116" s="43">
         <v>13</v>
       </c>
-      <c r="B116" s="54"/>
+      <c r="B116" s="45"/>
       <c r="C116" s="19" t="s">
         <v>0</v>
       </c>
@@ -6634,13 +6631,13 @@
       <c r="H116" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I116" s="52" t="str">
+      <c r="I116" s="46" t="str">
         <f>IF(H117&gt;H118,B117,B118)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117" s="50" t="s">
+      <c r="A117" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B117" s="14" t="s">
@@ -6670,10 +6667,10 @@
         <f>PRODUCT(C117:G117)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I117" s="52"/>
+      <c r="I117" s="46"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="51"/>
+      <c r="A118" s="44"/>
       <c r="B118" s="14" t="s">
         <v>2</v>
       </c>
@@ -6701,13 +6698,13 @@
         <f>PRODUCT(C118:G118)*$C$51</f>
         <v>1.6368382800000005E-2</v>
       </c>
-      <c r="I118" s="52"/>
+      <c r="I118" s="46"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119" s="53">
+      <c r="A119" s="43">
         <v>14</v>
       </c>
-      <c r="B119" s="54"/>
+      <c r="B119" s="45"/>
       <c r="C119" s="19" t="s">
         <v>0</v>
       </c>
@@ -6726,13 +6723,13 @@
       <c r="H119" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I119" s="52" t="str">
+      <c r="I119" s="46" t="str">
         <f>IF(H120&gt;H121,B120,B121)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A120" s="50" t="s">
+      <c r="A120" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B120" s="14" t="s">
@@ -6762,10 +6759,10 @@
         <f>PRODUCT(C120:G120)*$C$50</f>
         <v>9.7403644800000012E-3</v>
       </c>
-      <c r="I120" s="52"/>
+      <c r="I120" s="46"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A121" s="51"/>
+      <c r="A121" s="44"/>
       <c r="B121" s="14" t="s">
         <v>2</v>
       </c>
@@ -6793,13 +6790,13 @@
         <f>PRODUCT(C121:G121)*$C$51</f>
         <v>5.7289339800000012E-2</v>
       </c>
-      <c r="I121" s="52"/>
+      <c r="I121" s="46"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A122" s="53">
+      <c r="A122" s="43">
         <v>15</v>
       </c>
-      <c r="B122" s="54"/>
+      <c r="B122" s="45"/>
       <c r="C122" s="19" t="s">
         <v>0</v>
       </c>
@@ -6818,13 +6815,13 @@
       <c r="H122" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I122" s="52" t="str">
+      <c r="I122" s="46" t="str">
         <f>IF(H123&gt;H124,B123,B124)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A123" s="50" t="s">
+      <c r="A123" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B123" s="14" t="s">
@@ -6854,10 +6851,10 @@
         <f>PRODUCT(C123:G123)*$C$50</f>
         <v>2.7829612800000002E-3</v>
       </c>
-      <c r="I123" s="52"/>
+      <c r="I123" s="46"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A124" s="51"/>
+      <c r="A124" s="44"/>
       <c r="B124" s="14" t="s">
         <v>2</v>
       </c>
@@ -6885,13 +6882,13 @@
         <f>PRODUCT(C124:G124)*$C$51</f>
         <v>4.7741116500000014E-2</v>
       </c>
-      <c r="I124" s="52"/>
+      <c r="I124" s="46"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A125" s="53">
+      <c r="A125" s="43">
         <v>16</v>
       </c>
-      <c r="B125" s="54"/>
+      <c r="B125" s="45"/>
       <c r="C125" s="19" t="s">
         <v>1</v>
       </c>
@@ -6910,13 +6907,13 @@
       <c r="H125" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I125" s="52" t="str">
+      <c r="I125" s="46" t="str">
         <f>IF(H126&gt;H127,B126,B127)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A126" s="50" t="s">
+      <c r="A126" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B126" s="14" t="s">
@@ -6946,10 +6943,10 @@
         <f>PRODUCT(C126:G126)*$C$50</f>
         <v>1.9480728960000002E-2</v>
       </c>
-      <c r="I126" s="52"/>
+      <c r="I126" s="46"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A127" s="51"/>
+      <c r="A127" s="44"/>
       <c r="B127" s="14" t="s">
         <v>2</v>
       </c>
@@ -6977,13 +6974,13 @@
         <f>PRODUCT(C127:G127)*$C$51</f>
         <v>3.2736765600000009E-2</v>
       </c>
-      <c r="I127" s="52"/>
+      <c r="I127" s="46"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A128" s="53">
+      <c r="A128" s="43">
         <v>17</v>
       </c>
-      <c r="B128" s="54"/>
+      <c r="B128" s="45"/>
       <c r="C128" s="19" t="s">
         <v>1</v>
       </c>
@@ -7002,13 +6999,13 @@
       <c r="H128" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I128" s="52" t="str">
+      <c r="I128" s="46" t="str">
         <f>IF(H129&gt;H130,B129,B130)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A129" s="50" t="s">
+      <c r="A129" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B129" s="14" t="s">
@@ -7038,10 +7035,10 @@
         <f>PRODUCT(C129:G129)*$C$50</f>
         <v>5.5659225600000004E-3</v>
       </c>
-      <c r="I129" s="52"/>
+      <c r="I129" s="46"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A130" s="51"/>
+      <c r="A130" s="44"/>
       <c r="B130" s="14" t="s">
         <v>2</v>
       </c>
@@ -7069,13 +7066,13 @@
         <f>PRODUCT(C130:G130)*$C$51</f>
         <v>2.7280638000000006E-2</v>
       </c>
-      <c r="I130" s="52"/>
+      <c r="I130" s="46"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A131" s="53">
+      <c r="A131" s="43">
         <v>18</v>
       </c>
-      <c r="B131" s="54"/>
+      <c r="B131" s="45"/>
       <c r="C131" s="19" t="s">
         <v>0</v>
       </c>
@@ -7094,13 +7091,13 @@
       <c r="H131" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I131" s="52" t="str">
+      <c r="I131" s="46" t="str">
         <f>IF(H132&gt;H133,B132,B133)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A132" s="50" t="s">
+      <c r="A132" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B132" s="14" t="s">
@@ -7130,10 +7127,10 @@
         <f>PRODUCT(C132:G132)*$C$50</f>
         <v>9.7403644800000012E-3</v>
       </c>
-      <c r="I132" s="52"/>
+      <c r="I132" s="46"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A133" s="51"/>
+      <c r="A133" s="44"/>
       <c r="B133" s="14" t="s">
         <v>2</v>
       </c>
@@ -7161,13 +7158,13 @@
         <f>PRODUCT(C133:G133)*$C$51</f>
         <v>2.8644669900000006E-2</v>
       </c>
-      <c r="I133" s="52"/>
+      <c r="I133" s="46"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A134" s="53">
+      <c r="A134" s="43">
         <v>19</v>
       </c>
-      <c r="B134" s="53"/>
+      <c r="B134" s="43"/>
       <c r="C134" s="19" t="s">
         <v>0</v>
       </c>
@@ -7186,13 +7183,13 @@
       <c r="H134" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I134" s="60" t="str">
+      <c r="I134" s="42" t="str">
         <f>IF(H135&gt;H136,B135,B136)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A135" s="50" t="s">
+      <c r="A135" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B135" s="14" t="s">
@@ -7222,10 +7219,10 @@
         <f>PRODUCT(C135:G135)*$C$50</f>
         <v>1.2175455600000001E-2</v>
       </c>
-      <c r="I135" s="60"/>
+      <c r="I135" s="42"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A136" s="50"/>
+      <c r="A136" s="41"/>
       <c r="B136" s="14" t="s">
         <v>2</v>
       </c>
@@ -7253,13 +7250,13 @@
         <f>PRODUCT(C136:G136)*$C$51</f>
         <v>2.8644669900000008E-3</v>
       </c>
-      <c r="I136" s="60"/>
+      <c r="I136" s="42"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A137" s="53">
+      <c r="A137" s="43">
         <v>20</v>
       </c>
-      <c r="B137" s="54"/>
+      <c r="B137" s="45"/>
       <c r="C137" s="19" t="s">
         <v>1</v>
       </c>
@@ -7278,13 +7275,13 @@
       <c r="H137" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I137" s="55" t="str">
+      <c r="I137" s="47" t="str">
         <f>IF(H138&gt;H139,B138,B139)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A138" s="50" t="s">
+      <c r="A138" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B138" s="14" t="s">
@@ -7314,10 +7311,10 @@
         <f>PRODUCT(C138:G138)*$C$50</f>
         <v>2.4350911200000002E-2</v>
       </c>
-      <c r="I138" s="56"/>
+      <c r="I138" s="48"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A139" s="51"/>
+      <c r="A139" s="44"/>
       <c r="B139" s="14" t="s">
         <v>2</v>
       </c>
@@ -7345,11 +7342,91 @@
         <f>PRODUCT(C139:G139)*$C$51</f>
         <v>1.6368382800000002E-3</v>
       </c>
-      <c r="I139" s="57"/>
+      <c r="I139" s="49"/>
     </row>
     <row r="153" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="96">
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="A79:B80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="I80:I82"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G45"/>
+    <mergeCell ref="F28:G29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="A39:B40"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:G35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="I83:I85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="I86:I88"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="I89:I91"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="I92:I94"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="I95:I97"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="I98:I100"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="I101:I103"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="I107:I109"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="I137:I139"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="J67:K68"/>
+    <mergeCell ref="J69:K72"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="I131:I133"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="I125:I127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="I128:I130"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="I119:I121"/>
     <mergeCell ref="H28:K28"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="A135:A136"/>
@@ -7366,86 +7443,6 @@
     <mergeCell ref="I116:I118"/>
     <mergeCell ref="A117:A118"/>
     <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="I137:I139"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="J67:K68"/>
-    <mergeCell ref="J69:K72"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="I131:I133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="I125:I127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="I128:I130"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="I107:I109"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="I101:I103"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="I95:I97"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="I98:I100"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="I89:I91"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="I92:I94"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="I83:I85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="I86:I88"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A23:B24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:G35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:G29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="A39:B40"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:G40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:G45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="A79:B80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="I80:I82"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A1:A21 C2:D21">
@@ -7480,8 +7477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B7A5E7-0D1D-49AD-B6BD-E47ED560C8B9}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7513,462 +7510,462 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="68">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="68" t="s">
+      <c r="D2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="69">
-        <v>2</v>
-      </c>
-      <c r="B3" s="69" t="s">
+      <c r="A3" s="35">
+        <v>2</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="69" t="s">
+      <c r="D3" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="68">
-        <v>3</v>
-      </c>
-      <c r="B4" s="68" t="s">
+      <c r="A4" s="34">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="68" t="s">
+      <c r="D4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="69">
+      <c r="A5" s="35">
         <v>4</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="69" t="s">
+      <c r="D5" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="68">
+      <c r="A6" s="34">
         <v>5</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="68" t="s">
+      <c r="D6" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="68" t="s">
+      <c r="G6" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="69">
+      <c r="A7" s="35">
         <v>6</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="69" t="s">
+      <c r="D7" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="69" t="s">
+      <c r="G7" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="68">
+      <c r="A8" s="34">
         <v>7</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="68" t="s">
+      <c r="D8" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="69">
+      <c r="A9" s="35">
         <v>8</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="69" t="s">
+      <c r="D9" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="68">
+      <c r="A10" s="34">
         <v>9</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="68" t="s">
+      <c r="D10" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="68" t="s">
+      <c r="G10" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="69">
+      <c r="A11" s="35">
         <v>10</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="69" t="s">
+      <c r="D11" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="69" t="s">
+      <c r="G11" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="68">
+      <c r="A12" s="34">
         <v>11</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="68" t="s">
+      <c r="D12" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="68" t="s">
+      <c r="G12" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="69">
+      <c r="A13" s="35">
         <v>12</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="69" t="s">
+      <c r="D13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="69" t="s">
+      <c r="G13" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="68">
+      <c r="A14" s="34">
         <v>13</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="68" t="s">
+      <c r="D14" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="68" t="s">
+      <c r="G14" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="69">
+      <c r="A15" s="35">
         <v>14</v>
       </c>
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="69" t="s">
+      <c r="D15" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="69" t="s">
+      <c r="G15" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="68">
+      <c r="A16" s="34">
         <v>15</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="68" t="s">
+      <c r="D16" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="68" t="s">
+      <c r="G16" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="69">
+      <c r="A17" s="35">
         <v>16</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="69" t="s">
+      <c r="D17" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="69" t="s">
+      <c r="G17" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="68">
+      <c r="A18" s="34">
         <v>17</v>
       </c>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="68" t="s">
+      <c r="D18" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="68" t="s">
+      <c r="G18" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="69">
+      <c r="A19" s="35">
         <v>18</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="69" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="69" t="s">
+      <c r="D19" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="69" t="s">
+      <c r="G19" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="68">
+      <c r="A20" s="34">
         <v>19</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="68" t="s">
+      <c r="D20" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="68" t="s">
+      <c r="G20" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="70">
+      <c r="A21" s="29">
         <v>20</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="70" t="s">
+      <c r="D21" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="70" t="s">
+      <c r="G21" s="29" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7999,8 +7996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A02A39-F2B8-4A72-BE6A-2B6D7673FEB4}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8040,10 +8037,10 @@
       <c r="H1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="35"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -8278,34 +8275,34 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63" t="s">
+      <c r="B11" s="66"/>
+      <c r="C11" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="F11" s="62" t="s">
+      <c r="D11" s="68"/>
+      <c r="F11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="62"/>
-      <c r="H11" s="63" t="s">
+      <c r="G11" s="66"/>
+      <c r="H11" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="63"/>
+      <c r="I11" s="68"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
       <c r="H12" s="16" t="s">
         <v>3</v>
       </c>
@@ -8314,7 +8311,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="67" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -8324,9 +8321,9 @@
         <v>0.33</v>
       </c>
       <c r="D13" s="20">
-        <v>0.77</v>
-      </c>
-      <c r="F13" s="61" t="s">
+        <v>0.63</v>
+      </c>
+      <c r="F13" s="67" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="17" t="s">
@@ -8340,7 +8337,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="61"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="17" t="s">
         <v>1</v>
       </c>
@@ -8348,9 +8345,9 @@
         <v>0.66</v>
       </c>
       <c r="D14" s="20">
-        <v>0.44</v>
-      </c>
-      <c r="F14" s="61"/>
+        <v>0.36</v>
+      </c>
+      <c r="F14" s="67"/>
       <c r="G14" s="17" t="s">
         <v>13</v>
       </c>
@@ -8366,7 +8363,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="F15" s="61"/>
+      <c r="F15" s="67"/>
       <c r="G15" s="17" t="s">
         <v>14</v>
       </c>
@@ -8378,34 +8375,34 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="62"/>
-      <c r="C17" s="63" t="s">
+      <c r="B17" s="66"/>
+      <c r="C17" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="F17" s="62" t="s">
+      <c r="D17" s="68"/>
+      <c r="F17" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="63" t="s">
+      <c r="G17" s="66"/>
+      <c r="H17" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="68"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
       <c r="H18" s="16" t="s">
         <v>3</v>
       </c>
@@ -8414,7 +8411,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="67" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -8424,9 +8421,9 @@
         <v>0.77</v>
       </c>
       <c r="D19" s="20">
-        <v>0.09</v>
-      </c>
-      <c r="F19" s="61" t="s">
+        <v>0.54</v>
+      </c>
+      <c r="F19" s="67" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="17" t="s">
@@ -8440,7 +8437,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="61"/>
+      <c r="A20" s="67"/>
       <c r="B20" s="17" t="s">
         <v>2</v>
       </c>
@@ -8448,9 +8445,9 @@
         <v>0.22</v>
       </c>
       <c r="D20" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="F20" s="61"/>
+        <v>0.45</v>
+      </c>
+      <c r="F20" s="67"/>
       <c r="G20" s="17" t="s">
         <v>30</v>
       </c>
@@ -8468,23 +8465,23 @@
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="63" t="s">
+      <c r="B22" s="66"/>
+      <c r="C22" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="63"/>
+      <c r="D22" s="68"/>
       <c r="F22" s="20"/>
-      <c r="G22" s="64" t="s">
+      <c r="G22" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="64"/>
+      <c r="H22" s="69"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="62"/>
-      <c r="B23" s="62"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="16" t="s">
         <v>3</v>
       </c>
@@ -8495,16 +8492,15 @@
         <v>3</v>
       </c>
       <c r="G23" s="20">
-        <f>COUNTIF(Table3[Kelas],"Ya")</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H23" s="20">
         <f>G23/G25</f>
-        <v>0.42857142857142855</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="67" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -8520,16 +8516,15 @@
         <v>2</v>
       </c>
       <c r="G24" s="20">
-        <f>COUNTIF(Table3[Kelas],"Tidak")</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H24" s="20">
         <f>G24/G25</f>
-        <v>0.5714285714285714</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
+      <c r="A25" s="67"/>
       <c r="B25" s="17" t="s">
         <v>2</v>
       </c>
@@ -8543,7 +8538,8 @@
         <v>5</v>
       </c>
       <c r="G25" s="30">
-        <v>7</v>
+        <f>SUM(G23:G24)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -8606,10 +8602,10 @@
       <c r="H28" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J28" s="58" t="s">
+      <c r="J28" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="K28" s="58"/>
+      <c r="K28" s="50"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="29">
@@ -8636,8 +8632,8 @@
       <c r="H29" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="27">
@@ -8664,11 +8660,11 @@
       <c r="H30" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J30" s="67">
+      <c r="J30" s="63">
         <f>6/7*100</f>
         <v>85.714285714285708</v>
       </c>
-      <c r="K30" s="67"/>
+      <c r="K30" s="63"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="29">
@@ -8695,8 +8691,8 @@
       <c r="H31" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="27">
@@ -8723,8 +8719,8 @@
       <c r="H32" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="29">
@@ -8751,8 +8747,8 @@
       <c r="H33" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="27">
@@ -8781,10 +8777,10 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="36">
+      <c r="A36" s="56">
         <v>1</v>
       </c>
-      <c r="B36" s="36"/>
+      <c r="B36" s="56"/>
       <c r="C36" s="22" t="s">
         <v>17</v>
       </c>
@@ -8808,8 +8804,8 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="56"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="23" t="s">
         <v>1</v>
       </c>
@@ -8828,13 +8824,13 @@
       <c r="H37" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="52" t="str">
+      <c r="I37" s="46" t="str">
         <f>IF(H38&gt;H39,B38,B39)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B38" s="14" t="s">
@@ -8862,18 +8858,18 @@
       </c>
       <c r="H38" s="20">
         <f>PRODUCT(C38:G38)*$H$23</f>
-        <v>2.3191344000000003E-2</v>
-      </c>
-      <c r="I38" s="52"/>
+        <v>2.4350911200000002E-2</v>
+      </c>
+      <c r="I38" s="46"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="37"/>
+      <c r="A39" s="57"/>
       <c r="B39" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="20">
         <f>D14</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D39" s="20">
         <f>I14</f>
@@ -8885,7 +8881,7 @@
       </c>
       <c r="F39" s="20">
         <f>D19</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G39" s="20">
         <f>I19</f>
@@ -8893,15 +8889,15 @@
       </c>
       <c r="H39" s="20">
         <f>PRODUCT(C39:G39)*$H$24</f>
-        <v>3.4642079999999995E-4</v>
-      </c>
-      <c r="I39" s="52"/>
+        <v>1.6368382800000002E-3</v>
+      </c>
+      <c r="I39" s="46"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="65">
-        <v>2</v>
-      </c>
-      <c r="B40" s="66"/>
+      <c r="A40" s="64">
+        <v>2</v>
+      </c>
+      <c r="B40" s="65"/>
       <c r="C40" s="23" t="s">
         <v>0</v>
       </c>
@@ -8920,13 +8916,13 @@
       <c r="H40" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I40" s="52" t="str">
+      <c r="I40" s="46" t="str">
         <f>IF(H41&gt;H42,B41,B42)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="14" t="s">
@@ -8954,18 +8950,18 @@
       </c>
       <c r="H41" s="20">
         <f>PRODUCT(C41:G41)*$H$23</f>
-        <v>1.4494590000000002E-2</v>
-      </c>
-      <c r="I41" s="52"/>
+        <v>1.5219319500000002E-2</v>
+      </c>
+      <c r="I41" s="46"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="37"/>
+      <c r="A42" s="57"/>
       <c r="B42" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C42" s="20">
         <f>D13</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D42" s="20">
         <f>I13</f>
@@ -8977,7 +8973,7 @@
       </c>
       <c r="F42" s="20">
         <f>D19</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G42" s="20">
         <f>I20</f>
@@ -8985,15 +8981,15 @@
       </c>
       <c r="H42" s="20">
         <f>PRODUCT(C42:G42)*$H$24</f>
-        <v>6.9284159999999991E-4</v>
-      </c>
-      <c r="I42" s="52"/>
+        <v>3.2736765600000005E-3</v>
+      </c>
+      <c r="I42" s="46"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="65">
-        <v>3</v>
-      </c>
-      <c r="B43" s="66"/>
+      <c r="A43" s="64">
+        <v>3</v>
+      </c>
+      <c r="B43" s="65"/>
       <c r="C43" s="23" t="s">
         <v>1</v>
       </c>
@@ -9012,13 +9008,13 @@
       <c r="H43" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I43" s="52" t="str">
+      <c r="I43" s="46" t="str">
         <f>IF(H44&gt;H45,B44,B45)</f>
-        <v>Ya</v>
+        <v>Tidak</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -9046,18 +9042,18 @@
       </c>
       <c r="H44" s="20">
         <f>PRODUCT(C44:G44)*$H$23</f>
-        <v>4.6382688000000004E-3</v>
-      </c>
-      <c r="I44" s="52"/>
+        <v>4.8701822400000006E-3</v>
+      </c>
+      <c r="I44" s="46"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="37"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C45" s="20">
         <f>D14</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D45" s="20">
         <f>I15</f>
@@ -9069,7 +9065,7 @@
       </c>
       <c r="F45" s="20">
         <f>D19</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G45" s="20">
         <f>I19</f>
@@ -9077,15 +9073,15 @@
       </c>
       <c r="H45" s="20">
         <f>PRODUCT(C45:G45)*$H$24</f>
-        <v>2.3094719999999999E-3</v>
-      </c>
-      <c r="I45" s="52"/>
+        <v>1.0912255200000002E-2</v>
+      </c>
+      <c r="I45" s="46"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="65">
+      <c r="A46" s="64">
         <v>4</v>
       </c>
-      <c r="B46" s="66"/>
+      <c r="B46" s="65"/>
       <c r="C46" s="23" t="s">
         <v>1</v>
       </c>
@@ -9104,13 +9100,13 @@
       <c r="H46" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I46" s="43" t="str">
+      <c r="I46" s="52" t="str">
         <f>IF(H47&gt;H48,B47,B48)</f>
         <v>Ya</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B47" s="14" t="s">
@@ -9138,18 +9134,18 @@
       </c>
       <c r="H47" s="20">
         <f>PRODUCT(C47:G47)*$H$23</f>
-        <v>2.3191344000000003E-2</v>
-      </c>
-      <c r="I47" s="43"/>
+        <v>2.4350911200000002E-2</v>
+      </c>
+      <c r="I47" s="52"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="37"/>
+      <c r="A48" s="57"/>
       <c r="B48" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C48" s="20">
         <f>D14</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D48" s="20">
         <f>I14</f>
@@ -9161,7 +9157,7 @@
       </c>
       <c r="F48" s="20">
         <f>D19</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G48" s="20">
         <f>I19</f>
@@ -9169,15 +9165,15 @@
       </c>
       <c r="H48" s="20">
         <f>PRODUCT(C48:G48)*$H$24</f>
-        <v>3.4642079999999995E-4</v>
-      </c>
-      <c r="I48" s="43"/>
+        <v>1.6368382800000002E-3</v>
+      </c>
+      <c r="I48" s="52"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="65">
+      <c r="A49" s="64">
         <v>5</v>
       </c>
-      <c r="B49" s="66"/>
+      <c r="B49" s="65"/>
       <c r="C49" s="23" t="s">
         <v>0</v>
       </c>
@@ -9196,13 +9192,13 @@
       <c r="H49" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I49" s="52" t="str">
+      <c r="I49" s="46" t="str">
         <f>IF(H50&gt;H51,B50,B51)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B50" s="14" t="s">
@@ -9230,18 +9226,18 @@
       </c>
       <c r="H50" s="20">
         <f>PRODUCT(C50:G50)*$H$23</f>
-        <v>2.3191344000000002E-3</v>
-      </c>
-      <c r="I50" s="52"/>
+        <v>2.4350911200000003E-3</v>
+      </c>
+      <c r="I50" s="46"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="37"/>
+      <c r="A51" s="57"/>
       <c r="B51" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C51" s="20">
         <f>D13</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D51" s="20">
         <f>I15</f>
@@ -9253,7 +9249,7 @@
       </c>
       <c r="F51" s="20">
         <f>D19</f>
-        <v>0.09</v>
+        <v>0.54</v>
       </c>
       <c r="G51" s="20">
         <f>I19</f>
@@ -9261,15 +9257,15 @@
       </c>
       <c r="H51" s="20">
         <f>PRODUCT(C51:G51)*$H$24</f>
-        <v>4.0415759999999998E-3</v>
-      </c>
-      <c r="I51" s="52"/>
+        <v>1.9096446600000004E-2</v>
+      </c>
+      <c r="I51" s="46"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="65">
+      <c r="A52" s="64">
         <v>6</v>
       </c>
-      <c r="B52" s="66"/>
+      <c r="B52" s="65"/>
       <c r="C52" s="23" t="s">
         <v>1</v>
       </c>
@@ -9288,13 +9284,13 @@
       <c r="H52" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I52" s="52" t="str">
+      <c r="I52" s="46" t="str">
         <f>IF(H53&gt;H54,B53,B54)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B53" s="14" t="s">
@@ -9322,18 +9318,18 @@
       </c>
       <c r="H53" s="20">
         <f>PRODUCT(C53:G53)*$H$23</f>
-        <v>1.6565245714285713E-3</v>
-      </c>
-      <c r="I53" s="52"/>
+        <v>1.7393508E-3</v>
+      </c>
+      <c r="I53" s="46"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="37"/>
+      <c r="A54" s="57"/>
       <c r="B54" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C54" s="20">
         <f>D14</f>
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="D54" s="20">
         <f>I15</f>
@@ -9345,7 +9341,7 @@
       </c>
       <c r="F54" s="20">
         <f>D20</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="G54" s="20">
         <f>I20</f>
@@ -9353,15 +9349,15 @@
       </c>
       <c r="H54" s="20">
         <f>PRODUCT(C54:G54)*$H$24</f>
-        <v>1.3196982857142856E-2</v>
-      </c>
-      <c r="I54" s="52"/>
+        <v>5.1963119999999998E-3</v>
+      </c>
+      <c r="I54" s="46"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="65">
+      <c r="A55" s="64">
         <v>7</v>
       </c>
-      <c r="B55" s="66"/>
+      <c r="B55" s="65"/>
       <c r="C55" s="23" t="s">
         <v>0</v>
       </c>
@@ -9380,13 +9376,13 @@
       <c r="H55" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I55" s="52" t="str">
+      <c r="I55" s="46" t="str">
         <f>IF(H56&gt;H57,B56,B57)</f>
         <v>Tidak</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B56" s="14" t="s">
@@ -9414,18 +9410,18 @@
       </c>
       <c r="H56" s="20">
         <f>PRODUCT(C56:G56)*$H$23</f>
-        <v>2.6504393142857143E-3</v>
-      </c>
-      <c r="I56" s="52"/>
+        <v>2.7829612800000002E-3</v>
+      </c>
+      <c r="I56" s="46"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="37"/>
+      <c r="A57" s="57"/>
       <c r="B57" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C57" s="20">
         <f>D13</f>
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D57" s="20">
         <f>I13</f>
@@ -9437,7 +9433,7 @@
       </c>
       <c r="F57" s="20">
         <f>D20</f>
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="G57" s="20">
         <f>I19</f>
@@ -9445,37 +9441,12 @@
       </c>
       <c r="H57" s="20">
         <f>PRODUCT(C57:G57)*$H$24</f>
-        <v>0.12124728000000001</v>
-      </c>
-      <c r="I57" s="52"/>
+        <v>4.7741116500000014E-2</v>
+      </c>
+      <c r="I57" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="J28:K29"/>
-    <mergeCell ref="J30:K33"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="I43:I45"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="I55:I57"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A17:B18"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C22:D22"/>
@@ -9491,6 +9462,31 @@
     <mergeCell ref="F17:G18"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="I55:I57"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="J28:K29"/>
+    <mergeCell ref="J30:K33"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="I43:I45"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>